<commit_message>
added form3 mapping template
</commit_message>
<xml_diff>
--- a/parameters/mas_forms_tb_mapping.xlsx
+++ b/parameters/mas_forms_tb_mapping.xlsx
@@ -4,15 +4,16 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6320" firstSheet="1" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6315" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Agreed options" sheetId="4" state="hidden" r:id="rId1"/>
     <sheet name="Form 1 - TB mapping" sheetId="17" r:id="rId2"/>
     <sheet name="Form 1 - Qns for user inputs" sheetId="18" r:id="rId3"/>
-    <sheet name="AR AP listing template" sheetId="10" state="hidden" r:id="rId4"/>
-    <sheet name="AR AP ageing template" sheetId="11" state="hidden" r:id="rId5"/>
-    <sheet name="RPT template" sheetId="12" state="hidden" r:id="rId6"/>
+    <sheet name="Form 3 - TB mapping" sheetId="19" r:id="rId4"/>
+    <sheet name="AR AP listing template" sheetId="10" state="hidden" r:id="rId5"/>
+    <sheet name="AR AP ageing template" sheetId="11" state="hidden" r:id="rId6"/>
+    <sheet name="RPT template" sheetId="12" state="hidden" r:id="rId7"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -58,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="339" uniqueCount="284">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="445" uniqueCount="387">
   <si>
     <t>Form 1 - Statement of assets and liabilities</t>
   </si>
@@ -911,6 +912,319 @@
   </si>
   <si>
     <t>trade_cred_fund_mgmt</t>
+  </si>
+  <si>
+    <t>Previous year
+&lt;&lt;&lt;previous_fy&gt;&gt;&gt;
+$</t>
+  </si>
+  <si>
+    <t>Current year
+&lt;&lt;&lt;current_fy&gt;&gt;&gt;
+$</t>
+  </si>
+  <si>
+    <t xml:space="preserve">var_name </t>
+  </si>
+  <si>
+    <t>(1) Revenue -</t>
+  </si>
+  <si>
+    <t>(a) Brokerage and commission from:</t>
+  </si>
+  <si>
+    <t>(i) Exchange traded business</t>
+  </si>
+  <si>
+    <t>- Securities and units in a collective investment scheme</t>
+  </si>
+  <si>
+    <t>rev_broker_comm_etb_secs</t>
+  </si>
+  <si>
+    <t>- Futures and other derivatives contracts</t>
+  </si>
+  <si>
+    <t>rev_broker_comm_deriv</t>
+  </si>
+  <si>
+    <t>(ii) Non-exchange traded business</t>
+  </si>
+  <si>
+    <t>rev_broker_comm_non_etb_secs</t>
+  </si>
+  <si>
+    <t>- Over-the-counter derivatives contracts (excluding over-the-counter derivatives contracts where the underlying thing is a currency or currency index)</t>
+  </si>
+  <si>
+    <t>rev_broker_comm_non_etb_otcderiv</t>
+  </si>
+  <si>
+    <t>- Spot foreign exchange contracts for the purposes of leveraged foreign exchange trading and over-the-cunter derivatives contracts where the underlying thing is a currency or currency index</t>
+  </si>
+  <si>
+    <t>rev_broker_comm_spotforex</t>
+  </si>
+  <si>
+    <t>(b) Profit or loss from proprietary trading:</t>
+  </si>
+  <si>
+    <t>(i) Equity and equity derivatives</t>
+  </si>
+  <si>
+    <t>rev_pnl_proprtrade_eqderiv</t>
+  </si>
+  <si>
+    <t>(ii) Debt and debt derivatives</t>
+  </si>
+  <si>
+    <t>rev_pnl_proprtrade_debtderiv</t>
+  </si>
+  <si>
+    <t>(iii) Commodity and commodity derivatives</t>
+  </si>
+  <si>
+    <t>rev_pnl_proprtrade_commderiv</t>
+  </si>
+  <si>
+    <t>(iv) Foreign exchange</t>
+  </si>
+  <si>
+    <t>rev_pnl_proprtrade_forex</t>
+  </si>
+  <si>
+    <t>(v) Others</t>
+  </si>
+  <si>
+    <t>rev_pnl_proprtrade_others</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>(c) Underwriting commission</t>
+  </si>
+  <si>
+    <t>rev_underwrite_comm</t>
+  </si>
+  <si>
+    <t>(d) Portfolio management fees</t>
+  </si>
+  <si>
+    <t>(i) Management fees</t>
+  </si>
+  <si>
+    <t>rev_pfl_mgtfees_mgmt_fees</t>
+  </si>
+  <si>
+    <t>(ii) Advisory fees</t>
+  </si>
+  <si>
+    <t>rev_pfl_mgtfees_adv_fees</t>
+  </si>
+  <si>
+    <t>(e) Corporate finance fees from:</t>
+  </si>
+  <si>
+    <t>(i) Managing initial public offerings ("IPOs")</t>
+  </si>
+  <si>
+    <t>rev_corp_finfees_ipo</t>
+  </si>
+  <si>
+    <t>(ii) Others</t>
+  </si>
+  <si>
+    <t>rev_corp_finfees_others</t>
+  </si>
+  <si>
+    <t>(f) Trustee and custodian fees</t>
+  </si>
+  <si>
+    <t>rev_trust_custdn</t>
+  </si>
+  <si>
+    <t>(g) Commission rebates</t>
+  </si>
+  <si>
+    <t>rev_comm_rebates</t>
+  </si>
+  <si>
+    <t>(h) REIT management fees</t>
+  </si>
+  <si>
+    <t>(i) Base and performance fees</t>
+  </si>
+  <si>
+    <t>rev_reit_mgtfees_baseperf</t>
+  </si>
+  <si>
+    <t>(ii) Transaction fees (acquisitions &amp; disposals)</t>
+  </si>
+  <si>
+    <t>rev_reit_mgtfees_trans</t>
+  </si>
+  <si>
+    <t>(i) Fees for providing credit rating services</t>
+  </si>
+  <si>
+    <t>rev_crdrate_fees</t>
+  </si>
+  <si>
+    <t>(j) Interest:</t>
+  </si>
+  <si>
+    <t>(i) Product financing</t>
+  </si>
+  <si>
+    <t>rev_int_prodfin</t>
+  </si>
+  <si>
+    <t>rev_int_others</t>
+  </si>
+  <si>
+    <t>(k) Dividend</t>
+  </si>
+  <si>
+    <t>rev_dividend</t>
+  </si>
+  <si>
+    <t>(l) Other revenue (to specify if significant)</t>
+  </si>
+  <si>
+    <t>7410.100, 7410.200,7410.400</t>
+  </si>
+  <si>
+    <t>rev_other_revenue</t>
+  </si>
+  <si>
+    <t>Total Revenue</t>
+  </si>
+  <si>
+    <t>rev_total_revenue</t>
+  </si>
+  <si>
+    <t>(2) Less: Expenses -</t>
+  </si>
+  <si>
+    <t>(a) Bad debts written off</t>
+  </si>
+  <si>
+    <t>exp_bad_debts</t>
+  </si>
+  <si>
+    <t>(b) Provision for doubtful debts</t>
+  </si>
+  <si>
+    <t>exp_prov_dtf_debts</t>
+  </si>
+  <si>
+    <t>(c) Diminution in the value of specified products</t>
+  </si>
+  <si>
+    <t>exp_dimin</t>
+  </si>
+  <si>
+    <t>(d) Brokerage and commission from business in:</t>
+  </si>
+  <si>
+    <t>(i) Securities and units in a collective investment scheme</t>
+  </si>
+  <si>
+    <t>exp_broker_comm_secs</t>
+  </si>
+  <si>
+    <t>(ii) Futures and other derivatives contracts</t>
+  </si>
+  <si>
+    <t>exp_broker_comm_deriv</t>
+  </si>
+  <si>
+    <t>(iii) Others</t>
+  </si>
+  <si>
+    <t>exp_broker_comm_others</t>
+  </si>
+  <si>
+    <t>(e) Commission expense</t>
+  </si>
+  <si>
+    <t>(i) Other brokers/banks</t>
+  </si>
+  <si>
+    <t>exp_comm_expense_otherbroker</t>
+  </si>
+  <si>
+    <t>(ii) Agents (including remisiers)</t>
+  </si>
+  <si>
+    <t>exp_comm_expense_agents</t>
+  </si>
+  <si>
+    <t>(f) Interest expense</t>
+  </si>
+  <si>
+    <t>exp_int_expense</t>
+  </si>
+  <si>
+    <t>(g) Fee expense</t>
+  </si>
+  <si>
+    <t>exp_fee_expense</t>
+  </si>
+  <si>
+    <t>(h) Directors' remuneration</t>
+  </si>
+  <si>
+    <t>exp_dir_renum</t>
+  </si>
+  <si>
+    <t>(i) Salaries and other employment costs (excluding directors' remuneration)</t>
+  </si>
+  <si>
+    <t>exp_slry</t>
+  </si>
+  <si>
+    <t>(j) Other expenses (to specify if significant)</t>
+  </si>
+  <si>
+    <t>exp_other_expense</t>
+  </si>
+  <si>
+    <t>Total Expenses</t>
+  </si>
+  <si>
+    <t>exp_total_expense</t>
+  </si>
+  <si>
+    <t>Net profit before tax and extraordinary items</t>
+  </si>
+  <si>
+    <t>npbt</t>
+  </si>
+  <si>
+    <t>Less: Taxation</t>
+  </si>
+  <si>
+    <t>tax</t>
+  </si>
+  <si>
+    <t>Net profit after tax but before extraordinary items</t>
+  </si>
+  <si>
+    <t>npat_bef_extraord</t>
+  </si>
+  <si>
+    <t>Extraordinary items (net of tax)</t>
+  </si>
+  <si>
+    <t>extraord_items</t>
+  </si>
+  <si>
+    <t>Net profit after tax and extraordinary items for the year</t>
+  </si>
+  <si>
+    <t>npat</t>
   </si>
 </sst>
 </file>
@@ -1030,7 +1344,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="16">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -1235,6 +1549,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1243,7 +1577,7 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="13"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1336,6 +1670,56 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1630,19 +2014,19 @@
       <selection sqref="A1:A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>99</v>
       </c>
@@ -1663,17 +2047,17 @@
       <selection activeCell="H176" activeCellId="1" sqref="H173:H174 H176"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.26953125" style="6" customWidth="1"/>
-    <col min="2" max="3" width="5.453125" style="6" customWidth="1"/>
-    <col min="4" max="4" width="4.26953125" style="6" customWidth="1"/>
-    <col min="5" max="5" width="36.26953125" style="6" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="16.1796875" style="6" customWidth="1"/>
-    <col min="8" max="16384" width="9.1796875" style="6"/>
+    <col min="1" max="1" width="7.28515625" style="6" customWidth="1"/>
+    <col min="2" max="3" width="5.42578125" style="6" customWidth="1"/>
+    <col min="4" max="4" width="4.28515625" style="6" customWidth="1"/>
+    <col min="5" max="5" width="36.28515625" style="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="16.140625" style="6" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="26.5" thickBot="1" x14ac:dyDescent="0.65">
+    <row r="1" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
@@ -1682,7 +2066,7 @@
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
     </row>
-    <row r="2" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="25" t="s">
         <v>101</v>
       </c>
@@ -1693,7 +2077,7 @@
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
     </row>
-    <row r="3" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="27" t="s">
         <v>102</v>
       </c>
@@ -1704,7 +2088,7 @@
       <c r="D3" s="4"/>
       <c r="E3" s="4"/>
     </row>
-    <row r="4" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="27" t="s">
         <v>103</v>
       </c>
@@ -1715,7 +2099,7 @@
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
     </row>
-    <row r="5" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="29" t="s">
         <v>104</v>
       </c>
@@ -1724,7 +2108,7 @@
       <c r="D5" s="5"/>
       <c r="E5" s="5"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F7" s="6" t="s">
         <v>113</v>
       </c>
@@ -1735,7 +2119,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
         <v>125</v>
       </c>
@@ -1744,14 +2128,14 @@
       <c r="D8" s="8"/>
       <c r="E8" s="8"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B9" s="15" t="s">
         <v>126</v>
       </c>
       <c r="C9" s="15"/>
       <c r="D9" s="15"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C10" s="7" t="s">
         <v>18</v>
       </c>
@@ -1763,13 +2147,13 @@
         <v>153</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C11" s="7" t="s">
         <v>19</v>
       </c>
       <c r="D11" s="7"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D12" s="7" t="s">
         <v>20</v>
       </c>
@@ -1780,7 +2164,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D13" s="7" t="s">
         <v>21</v>
       </c>
@@ -1792,7 +2176,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C14" s="18" t="s">
         <v>1</v>
       </c>
@@ -1804,7 +2188,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C15" s="18" t="s">
         <v>2</v>
       </c>
@@ -1816,7 +2200,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C16" s="18" t="s">
         <v>3</v>
       </c>
@@ -1828,7 +2212,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C17" s="18" t="s">
         <v>4</v>
       </c>
@@ -1840,7 +2224,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C18" s="18" t="s">
         <v>5</v>
       </c>
@@ -1852,10 +2236,10 @@
         <v>160</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="G19" s="19"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="20" t="s">
         <v>6</v>
       </c>
@@ -1866,10 +2250,10 @@
         <v>252</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="G21" s="19"/>
     </row>
-    <row r="22" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" s="31" t="s">
         <v>7</v>
       </c>
@@ -1879,7 +2263,7 @@
       <c r="E22" s="8"/>
       <c r="G22" s="19"/>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B23" s="15" t="s">
         <v>8</v>
       </c>
@@ -1888,7 +2272,7 @@
       <c r="E23" s="15"/>
       <c r="G23" s="19"/>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C24" s="7" t="s">
         <v>22</v>
       </c>
@@ -1896,7 +2280,7 @@
       <c r="E24" s="7"/>
       <c r="G24" s="19"/>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D25" s="7" t="s">
         <v>9</v>
       </c>
@@ -1908,14 +2292,14 @@
         <v>161</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D26" s="7" t="s">
         <v>10</v>
       </c>
       <c r="E26" s="7"/>
       <c r="G26" s="19"/>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E27" s="7" t="s">
         <v>11</v>
       </c>
@@ -1927,7 +2311,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E28" s="7" t="s">
         <v>12</v>
       </c>
@@ -1939,7 +2323,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D29" s="7" t="s">
         <v>13</v>
       </c>
@@ -1952,7 +2336,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="17"/>
       <c r="D30" s="7" t="s">
         <v>14</v>
@@ -1966,7 +2350,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="17"/>
       <c r="D31" s="7" t="s">
         <v>15</v>
@@ -1975,7 +2359,7 @@
       <c r="F31" s="19"/>
       <c r="G31" s="19"/>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="17"/>
       <c r="E32" s="7" t="s">
         <v>23</v>
@@ -1988,7 +2372,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="17"/>
       <c r="E33" s="7" t="s">
         <v>16</v>
@@ -2001,7 +2385,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="17"/>
       <c r="D34" s="7" t="s">
         <v>17</v>
@@ -2010,7 +2394,7 @@
       <c r="F34" s="19"/>
       <c r="G34" s="19"/>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="17"/>
       <c r="E35" s="7" t="s">
         <v>11</v>
@@ -2023,7 +2407,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="17"/>
       <c r="E36" s="7" t="s">
         <v>12</v>
@@ -2036,7 +2420,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C37" s="7" t="s">
         <v>24</v>
       </c>
@@ -2045,7 +2429,7 @@
       <c r="F37" s="19"/>
       <c r="G37" s="19"/>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D38" s="7" t="s">
         <v>25</v>
       </c>
@@ -2053,7 +2437,7 @@
       <c r="F38" s="19"/>
       <c r="G38" s="19"/>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E39" s="7" t="s">
         <v>23</v>
       </c>
@@ -2065,7 +2449,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E40" s="7" t="s">
         <v>26</v>
       </c>
@@ -2077,7 +2461,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E41" s="7" t="s">
         <v>27</v>
       </c>
@@ -2089,7 +2473,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D42" s="7" t="s">
         <v>28</v>
       </c>
@@ -2102,7 +2486,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D43" s="7" t="s">
         <v>29</v>
       </c>
@@ -2115,14 +2499,14 @@
         <v>174</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C44" s="7"/>
       <c r="D44" s="7"/>
       <c r="E44" s="7"/>
       <c r="F44" s="19"/>
       <c r="G44" s="19"/>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C45" s="7" t="s">
         <v>30</v>
       </c>
@@ -2131,7 +2515,7 @@
       <c r="F45" s="19"/>
       <c r="G45" s="19"/>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D46" s="7" t="s">
         <v>25</v>
       </c>
@@ -2139,7 +2523,7 @@
       <c r="F46" s="19"/>
       <c r="G46" s="19"/>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E47" s="7" t="s">
         <v>23</v>
       </c>
@@ -2151,7 +2535,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E48" s="7" t="s">
         <v>16</v>
       </c>
@@ -2163,7 +2547,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="49" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="49" spans="3:8" x14ac:dyDescent="0.25">
       <c r="D49" s="7" t="s">
         <v>31</v>
       </c>
@@ -2176,7 +2560,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="50" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="50" spans="3:8" x14ac:dyDescent="0.25">
       <c r="D50" s="7" t="s">
         <v>29</v>
       </c>
@@ -2189,14 +2573,14 @@
         <v>178</v>
       </c>
     </row>
-    <row r="51" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="51" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C51" s="7"/>
       <c r="D51" s="7"/>
       <c r="E51" s="7"/>
       <c r="F51" s="19"/>
       <c r="G51" s="19"/>
     </row>
-    <row r="52" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="52" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C52" s="7" t="s">
         <v>32</v>
       </c>
@@ -2205,7 +2589,7 @@
       <c r="F52" s="19"/>
       <c r="G52" s="19"/>
     </row>
-    <row r="53" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="53" spans="3:8" x14ac:dyDescent="0.25">
       <c r="D53" s="7" t="s">
         <v>25</v>
       </c>
@@ -2213,7 +2597,7 @@
       <c r="F53" s="19"/>
       <c r="G53" s="19"/>
     </row>
-    <row r="54" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="54" spans="3:8" x14ac:dyDescent="0.25">
       <c r="E54" s="7" t="s">
         <v>23</v>
       </c>
@@ -2225,7 +2609,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="55" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="55" spans="3:8" x14ac:dyDescent="0.25">
       <c r="E55" s="7" t="s">
         <v>26</v>
       </c>
@@ -2237,7 +2621,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="56" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="56" spans="3:8" x14ac:dyDescent="0.25">
       <c r="E56" s="7" t="s">
         <v>27</v>
       </c>
@@ -2249,7 +2633,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="57" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="57" spans="3:8" x14ac:dyDescent="0.25">
       <c r="D57" s="7" t="s">
         <v>31</v>
       </c>
@@ -2262,7 +2646,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="58" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="58" spans="3:8" x14ac:dyDescent="0.25">
       <c r="D58" s="7" t="s">
         <v>29</v>
       </c>
@@ -2275,14 +2659,14 @@
         <v>183</v>
       </c>
     </row>
-    <row r="59" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="59" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C59" s="7"/>
       <c r="D59" s="7"/>
       <c r="E59" s="7"/>
       <c r="F59" s="19"/>
       <c r="G59" s="19"/>
     </row>
-    <row r="60" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="60" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C60" s="7" t="s">
         <v>33</v>
       </c>
@@ -2296,14 +2680,14 @@
         <v>184</v>
       </c>
     </row>
-    <row r="61" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="61" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C61" s="7"/>
       <c r="D61" s="7"/>
       <c r="E61" s="7"/>
       <c r="F61" s="19"/>
       <c r="G61" s="19"/>
     </row>
-    <row r="62" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="62" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C62" s="7" t="s">
         <v>34</v>
       </c>
@@ -2312,7 +2696,7 @@
       <c r="F62" s="19"/>
       <c r="G62" s="19"/>
     </row>
-    <row r="63" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="63" spans="3:8" x14ac:dyDescent="0.25">
       <c r="D63" s="7" t="s">
         <v>25</v>
       </c>
@@ -2320,7 +2704,7 @@
       <c r="F63" s="19"/>
       <c r="G63" s="19"/>
     </row>
-    <row r="64" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="64" spans="3:8" x14ac:dyDescent="0.25">
       <c r="E64" s="7" t="s">
         <v>23</v>
       </c>
@@ -2332,7 +2716,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="65" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="65" spans="3:8" x14ac:dyDescent="0.25">
       <c r="E65" s="7" t="s">
         <v>16</v>
       </c>
@@ -2344,7 +2728,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="66" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="66" spans="3:8" x14ac:dyDescent="0.25">
       <c r="D66" s="7" t="s">
         <v>35</v>
       </c>
@@ -2357,13 +2741,13 @@
         <v>187</v>
       </c>
     </row>
-    <row r="67" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="67" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C67" s="7"/>
       <c r="D67" s="7"/>
       <c r="E67" s="7"/>
       <c r="F67" s="19"/>
     </row>
-    <row r="68" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="68" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C68" s="7" t="s">
         <v>36</v>
       </c>
@@ -2377,13 +2761,13 @@
         <v>253</v>
       </c>
     </row>
-    <row r="69" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="69" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C69" s="7"/>
       <c r="D69" s="7"/>
       <c r="E69" s="7"/>
       <c r="F69" s="19"/>
     </row>
-    <row r="70" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="70" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C70" s="7" t="s">
         <v>138</v>
       </c>
@@ -2391,7 +2775,7 @@
       <c r="E70" s="7"/>
       <c r="F70" s="19"/>
     </row>
-    <row r="71" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="71" spans="3:8" x14ac:dyDescent="0.25">
       <c r="D71" s="7" t="s">
         <v>37</v>
       </c>
@@ -2403,7 +2787,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="72" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="72" spans="3:8" x14ac:dyDescent="0.25">
       <c r="D72" s="7" t="s">
         <v>38</v>
       </c>
@@ -2416,13 +2800,13 @@
         <v>189</v>
       </c>
     </row>
-    <row r="73" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="73" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C73" s="7"/>
       <c r="D73" s="7"/>
       <c r="E73" s="7"/>
       <c r="F73" s="19"/>
     </row>
-    <row r="74" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="74" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C74" s="7" t="s">
         <v>39</v>
       </c>
@@ -2430,7 +2814,7 @@
       <c r="E74" s="7"/>
       <c r="F74" s="19"/>
     </row>
-    <row r="75" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="75" spans="3:8" x14ac:dyDescent="0.25">
       <c r="D75" s="7" t="s">
         <v>40</v>
       </c>
@@ -2442,7 +2826,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="76" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="76" spans="3:8" x14ac:dyDescent="0.25">
       <c r="D76" s="7" t="s">
         <v>41</v>
       </c>
@@ -2455,13 +2839,13 @@
         <v>191</v>
       </c>
     </row>
-    <row r="77" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="77" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C77" s="7"/>
       <c r="D77" s="7"/>
       <c r="E77" s="7"/>
       <c r="F77" s="19"/>
     </row>
-    <row r="78" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="78" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C78" s="7" t="s">
         <v>42</v>
       </c>
@@ -2474,12 +2858,12 @@
         <v>192</v>
       </c>
     </row>
-    <row r="79" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="79" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C79" s="7"/>
       <c r="D79" s="7"/>
       <c r="E79" s="7"/>
     </row>
-    <row r="80" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="80" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C80" s="7" t="s">
         <v>43</v>
       </c>
@@ -2492,12 +2876,12 @@
         <v>193</v>
       </c>
     </row>
-    <row r="81" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="81" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C81" s="7"/>
       <c r="D81" s="7"/>
       <c r="E81" s="7"/>
     </row>
-    <row r="82" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="82" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C82" s="7" t="s">
         <v>44</v>
       </c>
@@ -2510,12 +2894,12 @@
         <v>194</v>
       </c>
     </row>
-    <row r="83" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="83" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C83" s="7"/>
       <c r="D83" s="7"/>
       <c r="E83" s="7"/>
     </row>
-    <row r="84" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="84" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C84" s="7" t="s">
         <v>45</v>
       </c>
@@ -2528,12 +2912,12 @@
         <v>195</v>
       </c>
     </row>
-    <row r="85" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="85" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C85" s="7"/>
       <c r="D85" s="7"/>
       <c r="E85" s="7"/>
     </row>
-    <row r="86" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="86" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C86" s="7" t="s">
         <v>46</v>
       </c>
@@ -2546,12 +2930,12 @@
         <v>196</v>
       </c>
     </row>
-    <row r="87" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="87" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C87" s="7"/>
       <c r="D87" s="7"/>
       <c r="E87" s="7"/>
     </row>
-    <row r="88" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="88" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C88" s="21" t="s">
         <v>47</v>
       </c>
@@ -2564,20 +2948,20 @@
         <v>254</v>
       </c>
     </row>
-    <row r="90" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="90" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B90" s="15" t="s">
         <v>127</v>
       </c>
       <c r="E90" s="15"/>
     </row>
-    <row r="91" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="91" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C91" s="7" t="s">
         <v>48</v>
       </c>
       <c r="D91" s="7"/>
       <c r="E91" s="7"/>
     </row>
-    <row r="92" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="92" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D92" s="7" t="s">
         <v>49</v>
       </c>
@@ -2589,7 +2973,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="93" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="93" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D93" s="7" t="s">
         <v>50</v>
       </c>
@@ -2602,13 +2986,13 @@
         <v>247</v>
       </c>
     </row>
-    <row r="94" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="94" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C94" s="7"/>
       <c r="D94" s="7"/>
       <c r="E94" s="7"/>
       <c r="F94" s="19"/>
     </row>
-    <row r="95" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="95" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C95" s="7" t="s">
         <v>51</v>
       </c>
@@ -2616,7 +3000,7 @@
       <c r="E95" s="7"/>
       <c r="F95" s="19"/>
     </row>
-    <row r="96" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="96" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D96" s="7" t="s">
         <v>40</v>
       </c>
@@ -2628,7 +3012,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="97" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="97" spans="3:8" x14ac:dyDescent="0.25">
       <c r="D97" s="7" t="s">
         <v>41</v>
       </c>
@@ -2641,12 +3025,12 @@
         <v>198</v>
       </c>
     </row>
-    <row r="98" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="98" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C98" s="7"/>
       <c r="D98" s="7"/>
       <c r="E98" s="7"/>
     </row>
-    <row r="99" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="99" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C99" s="7" t="s">
         <v>52</v>
       </c>
@@ -2659,12 +3043,12 @@
         <v>199</v>
       </c>
     </row>
-    <row r="100" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="100" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C100" s="7"/>
       <c r="D100" s="7"/>
       <c r="E100" s="7"/>
     </row>
-    <row r="101" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="101" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C101" s="7" t="s">
         <v>53</v>
       </c>
@@ -2677,13 +3061,13 @@
         <v>200</v>
       </c>
     </row>
-    <row r="102" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="102" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C102" s="7"/>
       <c r="D102" s="7"/>
       <c r="E102" s="7"/>
       <c r="G102" s="19"/>
     </row>
-    <row r="103" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="103" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C103" s="7" t="s">
         <v>54</v>
       </c>
@@ -2696,13 +3080,13 @@
         <v>201</v>
       </c>
     </row>
-    <row r="104" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="104" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C104" s="7"/>
       <c r="D104" s="7"/>
       <c r="E104" s="7"/>
       <c r="G104" s="19"/>
     </row>
-    <row r="105" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="105" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C105" s="7" t="s">
         <v>55</v>
       </c>
@@ -2715,12 +3099,12 @@
         <v>202</v>
       </c>
     </row>
-    <row r="106" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="106" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C106" s="7"/>
       <c r="D106" s="7"/>
       <c r="E106" s="7"/>
     </row>
-    <row r="107" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="107" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C107" s="7" t="s">
         <v>56</v>
       </c>
@@ -2733,12 +3117,12 @@
         <v>203</v>
       </c>
     </row>
-    <row r="108" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="108" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C108" s="7"/>
       <c r="D108" s="7"/>
       <c r="E108" s="7"/>
     </row>
-    <row r="109" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="109" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C109" s="7" t="s">
         <v>57</v>
       </c>
@@ -2751,12 +3135,12 @@
         <v>204</v>
       </c>
     </row>
-    <row r="110" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="110" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C110" s="7"/>
       <c r="D110" s="7"/>
       <c r="E110" s="7"/>
     </row>
-    <row r="111" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="111" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C111" s="21" t="s">
         <v>58</v>
       </c>
@@ -2769,12 +3153,12 @@
         <v>255</v>
       </c>
     </row>
-    <row r="112" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="112" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C112" s="7"/>
       <c r="D112" s="7"/>
       <c r="E112" s="7"/>
     </row>
-    <row r="113" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B113" s="22" t="s">
         <v>59</v>
       </c>
@@ -2787,7 +3171,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="115" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B115" s="20" t="s">
         <v>128</v>
       </c>
@@ -2800,12 +3184,12 @@
         <v>257</v>
       </c>
     </row>
-    <row r="117" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A117" s="20" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="118" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B118" s="15" t="s">
         <v>61</v>
       </c>
@@ -2813,14 +3197,14 @@
       <c r="D118" s="15"/>
       <c r="E118" s="15"/>
     </row>
-    <row r="119" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C119" s="7" t="s">
         <v>62</v>
       </c>
       <c r="D119" s="7"/>
       <c r="E119" s="7"/>
     </row>
-    <row r="120" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D120" s="7" t="s">
         <v>9</v>
       </c>
@@ -2832,13 +3216,13 @@
         <v>205</v>
       </c>
     </row>
-    <row r="121" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D121" s="7" t="s">
         <v>10</v>
       </c>
       <c r="E121" s="7"/>
     </row>
-    <row r="122" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E122" s="7" t="s">
         <v>11</v>
       </c>
@@ -2849,7 +3233,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="123" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E123" s="7" t="s">
         <v>12</v>
       </c>
@@ -2861,7 +3245,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="124" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D124" s="7" t="s">
         <v>63</v>
       </c>
@@ -2873,7 +3257,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="125" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D125" s="7" t="s">
         <v>64</v>
       </c>
@@ -2885,7 +3269,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="126" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D126" s="7" t="s">
         <v>65</v>
       </c>
@@ -2897,7 +3281,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="127" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D127" s="7" t="s">
         <v>66</v>
       </c>
@@ -2909,14 +3293,14 @@
         <v>211</v>
       </c>
     </row>
-    <row r="128" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D128" s="7" t="s">
         <v>67</v>
       </c>
       <c r="E128" s="7"/>
       <c r="G128" s="23"/>
     </row>
-    <row r="129" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="129" spans="3:8" x14ac:dyDescent="0.25">
       <c r="E129" s="7" t="s">
         <v>11</v>
       </c>
@@ -2927,7 +3311,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="130" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="130" spans="3:8" x14ac:dyDescent="0.25">
       <c r="E130" s="7" t="s">
         <v>12</v>
       </c>
@@ -2939,25 +3323,25 @@
         <v>213</v>
       </c>
     </row>
-    <row r="131" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="131" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C131" s="7"/>
       <c r="D131" s="7"/>
       <c r="E131" s="7"/>
     </row>
-    <row r="132" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="132" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C132" s="7" t="s">
         <v>68</v>
       </c>
       <c r="D132" s="7"/>
       <c r="E132" s="7"/>
     </row>
-    <row r="133" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="133" spans="3:8" x14ac:dyDescent="0.25">
       <c r="D133" s="7" t="s">
         <v>69</v>
       </c>
       <c r="E133" s="7"/>
     </row>
-    <row r="134" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="134" spans="3:8" x14ac:dyDescent="0.25">
       <c r="E134" s="7" t="s">
         <v>70</v>
       </c>
@@ -2968,7 +3352,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="135" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="135" spans="3:8" x14ac:dyDescent="0.25">
       <c r="E135" s="7" t="s">
         <v>16</v>
       </c>
@@ -2980,7 +3364,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="136" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="136" spans="3:8" x14ac:dyDescent="0.25">
       <c r="D136" s="7" t="s">
         <v>71</v>
       </c>
@@ -2992,7 +3376,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="137" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="137" spans="3:8" x14ac:dyDescent="0.25">
       <c r="D137" s="7" t="s">
         <v>29</v>
       </c>
@@ -3004,20 +3388,20 @@
         <v>217</v>
       </c>
     </row>
-    <row r="138" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="138" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C138" s="7"/>
       <c r="D138" s="7"/>
       <c r="E138" s="7"/>
       <c r="G138" s="19"/>
     </row>
-    <row r="139" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="139" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C139" s="7" t="s">
         <v>72</v>
       </c>
       <c r="D139" s="7"/>
       <c r="E139" s="7"/>
     </row>
-    <row r="140" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="140" spans="3:8" x14ac:dyDescent="0.25">
       <c r="D140" s="7" t="s">
         <v>69</v>
       </c>
@@ -3029,7 +3413,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="141" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="141" spans="3:8" x14ac:dyDescent="0.25">
       <c r="D141" s="7" t="s">
         <v>73</v>
       </c>
@@ -3041,7 +3425,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="142" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="142" spans="3:8" x14ac:dyDescent="0.25">
       <c r="D142" s="7" t="s">
         <v>29</v>
       </c>
@@ -3053,25 +3437,25 @@
         <v>220</v>
       </c>
     </row>
-    <row r="143" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="143" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C143" s="7"/>
       <c r="D143" s="7"/>
       <c r="E143" s="7"/>
     </row>
-    <row r="144" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="144" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C144" s="7" t="s">
         <v>74</v>
       </c>
       <c r="D144" s="7"/>
       <c r="E144" s="7"/>
     </row>
-    <row r="145" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="145" spans="3:8" x14ac:dyDescent="0.25">
       <c r="D145" s="7" t="s">
         <v>69</v>
       </c>
       <c r="E145" s="7"/>
     </row>
-    <row r="146" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="146" spans="3:8" x14ac:dyDescent="0.25">
       <c r="E146" s="7" t="s">
         <v>70</v>
       </c>
@@ -3082,7 +3466,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="147" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="147" spans="3:8" x14ac:dyDescent="0.25">
       <c r="E147" s="7" t="s">
         <v>16</v>
       </c>
@@ -3094,7 +3478,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="148" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="148" spans="3:8" x14ac:dyDescent="0.25">
       <c r="D148" s="7" t="s">
         <v>71</v>
       </c>
@@ -3106,7 +3490,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="149" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="149" spans="3:8" x14ac:dyDescent="0.25">
       <c r="D149" s="7" t="s">
         <v>29</v>
       </c>
@@ -3118,12 +3502,12 @@
         <v>224</v>
       </c>
     </row>
-    <row r="150" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="150" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C150" s="7"/>
       <c r="D150" s="7"/>
       <c r="E150" s="7"/>
     </row>
-    <row r="151" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="151" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C151" s="7" t="s">
         <v>75</v>
       </c>
@@ -3136,12 +3520,12 @@
         <v>225</v>
       </c>
     </row>
-    <row r="152" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="152" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C152" s="7"/>
       <c r="D152" s="7"/>
       <c r="E152" s="7"/>
     </row>
-    <row r="153" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="153" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C153" s="7" t="s">
         <v>76</v>
       </c>
@@ -3154,12 +3538,12 @@
         <v>226</v>
       </c>
     </row>
-    <row r="154" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="154" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C154" s="7"/>
       <c r="D154" s="7"/>
       <c r="E154" s="7"/>
     </row>
-    <row r="155" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="155" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C155" s="7" t="s">
         <v>77</v>
       </c>
@@ -3172,7 +3556,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="156" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="156" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C156" s="7" t="s">
         <v>115</v>
       </c>
@@ -3187,7 +3571,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="157" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="157" spans="3:8" x14ac:dyDescent="0.25">
       <c r="D157" s="7" t="s">
         <v>137</v>
       </c>
@@ -3199,7 +3583,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="158" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="158" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C158" s="7" t="s">
         <v>78</v>
       </c>
@@ -3212,19 +3596,19 @@
         <v>259</v>
       </c>
     </row>
-    <row r="159" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="159" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C159" s="7"/>
       <c r="D159" s="7"/>
       <c r="E159" s="7"/>
     </row>
-    <row r="160" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="160" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C160" s="7" t="s">
         <v>138</v>
       </c>
       <c r="D160" s="7"/>
       <c r="E160" s="7"/>
     </row>
-    <row r="161" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="161" spans="3:8" x14ac:dyDescent="0.25">
       <c r="D161" s="7" t="s">
         <v>79</v>
       </c>
@@ -3236,7 +3620,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="162" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="162" spans="3:8" x14ac:dyDescent="0.25">
       <c r="D162" s="7" t="s">
         <v>80</v>
       </c>
@@ -3248,7 +3632,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="163" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="163" spans="3:8" x14ac:dyDescent="0.25">
       <c r="D163" s="7" t="s">
         <v>81</v>
       </c>
@@ -3261,12 +3645,12 @@
         <v>230</v>
       </c>
     </row>
-    <row r="164" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="164" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C164" s="7"/>
       <c r="D164" s="7"/>
       <c r="E164" s="7"/>
     </row>
-    <row r="165" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="165" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C165" s="7" t="s">
         <v>139</v>
       </c>
@@ -3279,19 +3663,19 @@
         <v>232</v>
       </c>
     </row>
-    <row r="166" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="166" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C166" s="7"/>
       <c r="D166" s="7"/>
       <c r="E166" s="7"/>
     </row>
-    <row r="167" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="167" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C167" s="7" t="s">
         <v>82</v>
       </c>
       <c r="D167" s="7"/>
       <c r="E167" s="7"/>
     </row>
-    <row r="168" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="168" spans="3:8" x14ac:dyDescent="0.25">
       <c r="D168" s="7" t="s">
         <v>79</v>
       </c>
@@ -3303,7 +3687,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="169" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="169" spans="3:8" x14ac:dyDescent="0.25">
       <c r="D169" s="7" t="s">
         <v>83</v>
       </c>
@@ -3315,7 +3699,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="170" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="170" spans="3:8" x14ac:dyDescent="0.25">
       <c r="D170" s="7" t="s">
         <v>81</v>
       </c>
@@ -3328,19 +3712,19 @@
         <v>235</v>
       </c>
     </row>
-    <row r="171" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="171" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C171" s="7"/>
       <c r="D171" s="7"/>
       <c r="E171" s="7"/>
     </row>
-    <row r="172" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="172" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C172" s="7" t="s">
         <v>84</v>
       </c>
       <c r="D172" s="7"/>
       <c r="E172" s="7"/>
     </row>
-    <row r="173" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="173" spans="3:8" x14ac:dyDescent="0.25">
       <c r="D173" s="7" t="s">
         <v>40</v>
       </c>
@@ -3352,7 +3736,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="174" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="174" spans="3:8" x14ac:dyDescent="0.25">
       <c r="D174" s="7" t="s">
         <v>41</v>
       </c>
@@ -3365,12 +3749,12 @@
         <v>237</v>
       </c>
     </row>
-    <row r="175" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="175" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C175" s="7"/>
       <c r="D175" s="7"/>
       <c r="E175" s="7"/>
     </row>
-    <row r="176" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="176" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C176" s="7" t="s">
         <v>85</v>
       </c>
@@ -3383,12 +3767,12 @@
         <v>238</v>
       </c>
     </row>
-    <row r="177" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="177" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C177" s="7"/>
       <c r="D177" s="7"/>
       <c r="E177" s="7"/>
     </row>
-    <row r="178" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="178" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C178" s="7" t="s">
         <v>86</v>
       </c>
@@ -3401,19 +3785,19 @@
         <v>239</v>
       </c>
     </row>
-    <row r="179" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="179" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C179" s="7"/>
       <c r="D179" s="7"/>
       <c r="E179" s="7"/>
     </row>
-    <row r="180" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="180" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C180" s="7" t="s">
         <v>87</v>
       </c>
       <c r="D180" s="7"/>
       <c r="E180" s="7"/>
     </row>
-    <row r="181" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="181" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D181" s="7" t="s">
         <v>88</v>
       </c>
@@ -3425,7 +3809,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="182" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="182" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D182" s="7" t="s">
         <v>89</v>
       </c>
@@ -3437,7 +3821,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="183" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="183" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D183" s="7" t="s">
         <v>81</v>
       </c>
@@ -3450,12 +3834,12 @@
         <v>242</v>
       </c>
     </row>
-    <row r="184" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="184" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C184" s="7"/>
       <c r="D184" s="7"/>
       <c r="E184" s="7"/>
     </row>
-    <row r="185" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="185" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C185" s="21" t="s">
         <v>90</v>
       </c>
@@ -3468,7 +3852,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="187" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="187" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B187" s="15" t="s">
         <v>129</v>
       </c>
@@ -3476,7 +3860,7 @@
       <c r="D187" s="15"/>
       <c r="E187" s="15"/>
     </row>
-    <row r="188" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="188" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C188" s="7" t="s">
         <v>140</v>
       </c>
@@ -3489,19 +3873,19 @@
         <v>243</v>
       </c>
     </row>
-    <row r="189" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="189" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C189" s="7"/>
       <c r="D189" s="7"/>
       <c r="E189" s="7"/>
     </row>
-    <row r="190" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="190" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C190" s="7" t="s">
         <v>91</v>
       </c>
       <c r="D190" s="7"/>
       <c r="E190" s="7"/>
     </row>
-    <row r="191" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="191" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D191" s="7" t="s">
         <v>49</v>
       </c>
@@ -3513,7 +3897,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="192" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="192" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D192" s="7" t="s">
         <v>50</v>
       </c>
@@ -3526,12 +3910,12 @@
         <v>245</v>
       </c>
     </row>
-    <row r="193" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="193" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C193" s="7"/>
       <c r="D193" s="7"/>
       <c r="E193" s="7"/>
     </row>
-    <row r="194" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="194" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C194" s="7" t="s">
         <v>92</v>
       </c>
@@ -3544,12 +3928,12 @@
         <v>248</v>
       </c>
     </row>
-    <row r="195" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="195" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C195" s="7"/>
       <c r="D195" s="7"/>
       <c r="E195" s="7"/>
     </row>
-    <row r="196" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="196" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C196" s="7" t="s">
         <v>93</v>
       </c>
@@ -3562,12 +3946,12 @@
         <v>249</v>
       </c>
     </row>
-    <row r="197" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="197" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C197" s="7"/>
       <c r="D197" s="7"/>
       <c r="E197" s="7"/>
     </row>
-    <row r="198" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="198" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C198" s="7" t="s">
         <v>94</v>
       </c>
@@ -3580,12 +3964,12 @@
         <v>250</v>
       </c>
     </row>
-    <row r="199" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="199" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C199" s="7"/>
       <c r="D199" s="7"/>
       <c r="E199" s="7"/>
     </row>
-    <row r="200" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="200" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C200" s="21" t="s">
         <v>95</v>
       </c>
@@ -3598,13 +3982,13 @@
         <v>261</v>
       </c>
     </row>
-    <row r="201" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="201" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B201" s="21"/>
       <c r="C201" s="21"/>
       <c r="D201" s="21"/>
       <c r="E201" s="21"/>
     </row>
-    <row r="202" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="202" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B202" s="22" t="s">
         <v>124</v>
       </c>
@@ -3618,17 +4002,17 @@
         <v>262</v>
       </c>
     </row>
-    <row r="204" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="204" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A204" s="20" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="206" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="206" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A206" s="18" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="207" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="207" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B207" s="7" t="s">
         <v>142</v>
       </c>
@@ -3637,7 +4021,7 @@
       <c r="E207" s="7"/>
       <c r="G207" s="3"/>
     </row>
-    <row r="208" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="208" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B208" s="7" t="s">
         <v>143</v>
       </c>
@@ -3646,7 +4030,7 @@
       <c r="E208" s="7"/>
       <c r="G208" s="24"/>
     </row>
-    <row r="209" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="209" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B209" s="7" t="s">
         <v>144</v>
       </c>
@@ -3655,54 +4039,54 @@
       <c r="E209" s="7"/>
       <c r="G209" s="24"/>
     </row>
-    <row r="210" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="210" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B210" s="3"/>
       <c r="C210" s="17"/>
       <c r="D210" s="17"/>
       <c r="E210" s="17"/>
       <c r="G210" s="24"/>
     </row>
-    <row r="211" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="211" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B211" s="24"/>
       <c r="C211" s="17"/>
       <c r="D211" s="17"/>
       <c r="E211" s="17"/>
       <c r="G211" s="24"/>
     </row>
-    <row r="212" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="212" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B212" s="24"/>
       <c r="C212" s="17"/>
       <c r="D212" s="17"/>
       <c r="E212" s="17"/>
       <c r="G212" s="24"/>
     </row>
-    <row r="213" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="213" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B213" s="24"/>
       <c r="C213" s="17"/>
       <c r="D213" s="17"/>
       <c r="E213" s="17"/>
       <c r="G213" s="24"/>
     </row>
-    <row r="214" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="214" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B214" s="24"/>
       <c r="C214" s="17"/>
       <c r="D214" s="17"/>
       <c r="E214" s="17"/>
       <c r="G214" s="24"/>
     </row>
-    <row r="215" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="215" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B215" s="24"/>
       <c r="C215" s="17"/>
       <c r="D215" s="17"/>
       <c r="E215" s="17"/>
       <c r="G215" s="24"/>
     </row>
-    <row r="217" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="217" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A217" s="18" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="218" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="218" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B218" s="7" t="s">
         <v>145</v>
       </c>
@@ -3711,7 +4095,7 @@
       <c r="E218" s="7"/>
       <c r="F218" s="3"/>
     </row>
-    <row r="219" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="219" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B219" s="7" t="s">
         <v>97</v>
       </c>
@@ -3721,13 +4105,13 @@
       <c r="F219" s="3"/>
       <c r="G219" s="3"/>
     </row>
-    <row r="220" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="220" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B220" s="7"/>
       <c r="C220" s="7"/>
       <c r="D220" s="7"/>
       <c r="E220" s="7"/>
     </row>
-    <row r="221" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="221" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B221" s="7" t="s">
         <v>146</v>
       </c>
@@ -3736,7 +4120,7 @@
       <c r="E221" s="7"/>
       <c r="F221" s="3"/>
     </row>
-    <row r="222" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="222" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B222" s="7" t="s">
         <v>97</v>
       </c>
@@ -3746,7 +4130,7 @@
       <c r="F222" s="3"/>
       <c r="G222" s="3"/>
     </row>
-    <row r="223" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="223" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B223" s="7" t="s">
         <v>144</v>
       </c>
@@ -3754,54 +4138,54 @@
       <c r="D223" s="7"/>
       <c r="E223" s="7"/>
     </row>
-    <row r="224" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="224" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B224" s="3"/>
       <c r="C224" s="17"/>
       <c r="D224" s="17"/>
       <c r="E224" s="17"/>
       <c r="G224" s="24"/>
     </row>
-    <row r="225" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="225" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B225" s="24"/>
       <c r="C225" s="17"/>
       <c r="D225" s="17"/>
       <c r="E225" s="17"/>
       <c r="G225" s="24"/>
     </row>
-    <row r="226" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="226" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B226" s="24"/>
       <c r="C226" s="17"/>
       <c r="D226" s="17"/>
       <c r="E226" s="17"/>
       <c r="G226" s="24"/>
     </row>
-    <row r="227" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="227" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B227" s="24"/>
       <c r="C227" s="17"/>
       <c r="D227" s="17"/>
       <c r="E227" s="17"/>
       <c r="G227" s="24"/>
     </row>
-    <row r="228" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="228" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B228" s="24"/>
       <c r="C228" s="17"/>
       <c r="D228" s="17"/>
       <c r="E228" s="17"/>
       <c r="G228" s="24"/>
     </row>
-    <row r="229" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="229" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B229" s="24"/>
       <c r="C229" s="17"/>
       <c r="D229" s="17"/>
       <c r="E229" s="17"/>
       <c r="G229" s="24"/>
     </row>
-    <row r="231" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="231" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A231" s="18" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="232" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="232" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B232" s="7" t="s">
         <v>147</v>
       </c>
@@ -3810,7 +4194,7 @@
       <c r="E232" s="7"/>
       <c r="G232" s="3"/>
     </row>
-    <row r="233" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="233" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B233" s="7" t="s">
         <v>148</v>
       </c>
@@ -3819,7 +4203,7 @@
       <c r="E233" s="7"/>
       <c r="G233" s="3"/>
     </row>
-    <row r="234" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="234" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B234" s="7" t="s">
         <v>149</v>
       </c>
@@ -3828,12 +4212,12 @@
       <c r="E234" s="7"/>
       <c r="G234" s="3"/>
     </row>
-    <row r="236" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="236" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A236" s="18" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="237" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="237" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B237" s="7" t="s">
         <v>150</v>
       </c>
@@ -3842,7 +4226,7 @@
       <c r="E237" s="7"/>
       <c r="G237" s="3"/>
     </row>
-    <row r="238" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="238" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B238" s="7" t="s">
         <v>151</v>
       </c>
@@ -3872,27 +4256,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34.453125" customWidth="1"/>
-    <col min="2" max="2" width="54.26953125" customWidth="1"/>
+    <col min="1" max="1" width="34.42578125" customWidth="1"/>
+    <col min="2" max="2" width="54.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>265</v>
       </c>
@@ -3903,7 +4287,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>277</v>
       </c>
@@ -3914,7 +4298,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>253</v>
       </c>
@@ -3925,7 +4309,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>283</v>
       </c>
@@ -3936,7 +4320,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>282</v>
       </c>
@@ -3947,7 +4331,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>281</v>
       </c>
@@ -3958,7 +4342,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>280</v>
       </c>
@@ -3969,7 +4353,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>278</v>
       </c>
@@ -3980,7 +4364,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>279</v>
       </c>
@@ -4002,69 +4386,882 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A4:G99"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="82" workbookViewId="0">
+      <selection activeCell="D54" sqref="D54"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.1796875" customWidth="1"/>
-    <col min="3" max="3" width="20.1796875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="8.7265625" style="1"/>
+    <col min="1" max="1" width="9.140625" style="32"/>
+    <col min="2" max="2" width="4.85546875" style="32" customWidth="1"/>
+    <col min="3" max="3" width="8.42578125" style="32" customWidth="1"/>
+    <col min="4" max="4" width="86.5703125" style="32" customWidth="1"/>
+    <col min="5" max="5" width="21" customWidth="1"/>
+    <col min="6" max="6" width="21.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>113</v>
-      </c>
-    </row>
+    <row r="4" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="E4" s="33" t="s">
+        <v>284</v>
+      </c>
+      <c r="F4" s="33" t="s">
+        <v>285</v>
+      </c>
+      <c r="G4" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="32" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B6" s="34" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C7" s="34" t="s">
+        <v>289</v>
+      </c>
+      <c r="D7" s="34"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D8" s="35" t="s">
+        <v>290</v>
+      </c>
+      <c r="E8" s="36"/>
+      <c r="F8" s="36"/>
+      <c r="G8" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D9" s="35" t="s">
+        <v>292</v>
+      </c>
+      <c r="E9" s="36"/>
+      <c r="F9" s="36"/>
+      <c r="G9" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C10" s="35"/>
+      <c r="D10" s="35"/>
+      <c r="E10" s="37"/>
+      <c r="F10" s="37"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C11" s="38" t="s">
+        <v>294</v>
+      </c>
+      <c r="D11" s="38"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D12" s="39" t="s">
+        <v>290</v>
+      </c>
+      <c r="E12" s="36"/>
+      <c r="F12" s="36"/>
+      <c r="G12" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="D13" s="39" t="s">
+        <v>296</v>
+      </c>
+      <c r="E13" s="36"/>
+      <c r="F13" s="36"/>
+      <c r="G13" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="D14" s="39" t="s">
+        <v>298</v>
+      </c>
+      <c r="E14" s="36"/>
+      <c r="F14" s="36"/>
+      <c r="G14" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C15" s="40"/>
+      <c r="D15" s="40"/>
+      <c r="E15" s="37"/>
+      <c r="F15" s="37"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B16" s="41" t="s">
+        <v>300</v>
+      </c>
+      <c r="D16" s="41"/>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C17" s="40" t="s">
+        <v>301</v>
+      </c>
+      <c r="D17" s="40"/>
+      <c r="E17" s="36"/>
+      <c r="F17" s="36"/>
+      <c r="G17" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C18" s="40" t="s">
+        <v>303</v>
+      </c>
+      <c r="D18" s="40"/>
+      <c r="E18" s="42"/>
+      <c r="F18" s="42"/>
+      <c r="G18" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C19" s="40" t="s">
+        <v>305</v>
+      </c>
+      <c r="D19" s="40"/>
+      <c r="E19" s="42"/>
+      <c r="F19" s="42"/>
+      <c r="G19" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C20" s="40" t="s">
+        <v>307</v>
+      </c>
+      <c r="D20" s="40"/>
+      <c r="E20" s="42"/>
+      <c r="F20" s="42"/>
+      <c r="G20" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C21" s="38" t="s">
+        <v>309</v>
+      </c>
+      <c r="D21" s="38"/>
+      <c r="E21" s="42"/>
+      <c r="F21" s="42"/>
+      <c r="G21" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C22" s="38"/>
+      <c r="D22" s="38" t="s">
+        <v>311</v>
+      </c>
+      <c r="E22" s="37"/>
+      <c r="F22" s="37"/>
+    </row>
+    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B23" s="38" t="s">
+        <v>312</v>
+      </c>
+      <c r="D23" s="38"/>
+      <c r="E23" s="36"/>
+      <c r="F23" s="36"/>
+      <c r="G23" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C24" s="38"/>
+      <c r="D24" s="38"/>
+      <c r="E24" s="37"/>
+      <c r="F24" s="37"/>
+    </row>
+    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B25" s="38" t="s">
+        <v>314</v>
+      </c>
+      <c r="D25" s="38"/>
+      <c r="E25" s="37"/>
+      <c r="F25" s="37"/>
+    </row>
+    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C26" s="38" t="s">
+        <v>315</v>
+      </c>
+      <c r="D26" s="38"/>
+      <c r="E26" s="43">
+        <v>7000.1</v>
+      </c>
+      <c r="F26" s="43">
+        <v>7000.1</v>
+      </c>
+      <c r="G26" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C27" s="38" t="s">
+        <v>317</v>
+      </c>
+      <c r="D27" s="38"/>
+      <c r="E27" s="44">
+        <v>7000.2</v>
+      </c>
+      <c r="F27" s="44">
+        <v>7000.2</v>
+      </c>
+      <c r="G27" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="28" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C28" s="38"/>
+      <c r="D28" s="38"/>
+      <c r="E28" s="37"/>
+      <c r="F28" s="37"/>
+    </row>
+    <row r="29" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B29" s="38" t="s">
+        <v>319</v>
+      </c>
+      <c r="D29" s="38"/>
+      <c r="E29" s="37"/>
+      <c r="F29" s="37"/>
+    </row>
+    <row r="30" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C30" s="38" t="s">
+        <v>320</v>
+      </c>
+      <c r="D30" s="38"/>
+      <c r="E30" s="45">
+        <v>7000.4</v>
+      </c>
+      <c r="F30" s="45">
+        <v>7000.4</v>
+      </c>
+      <c r="G30" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="31" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C31" s="38" t="s">
+        <v>322</v>
+      </c>
+      <c r="D31" s="38"/>
+      <c r="E31" s="44">
+        <v>7000.5</v>
+      </c>
+      <c r="F31" s="44">
+        <v>7000.5</v>
+      </c>
+      <c r="G31" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="32" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C32" s="38"/>
+      <c r="D32" s="38"/>
+      <c r="E32" s="37"/>
+      <c r="F32" s="37"/>
+    </row>
+    <row r="33" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B33" s="38" t="s">
+        <v>324</v>
+      </c>
+      <c r="D33" s="38"/>
+      <c r="E33" s="45">
+        <v>7000.6</v>
+      </c>
+      <c r="F33" s="45">
+        <v>7000.6</v>
+      </c>
+      <c r="G33" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="34" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C34" s="38"/>
+      <c r="D34" s="38"/>
+      <c r="E34" s="37"/>
+      <c r="F34" s="37"/>
+    </row>
+    <row r="35" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B35" s="38" t="s">
+        <v>326</v>
+      </c>
+      <c r="D35" s="38"/>
+      <c r="E35" s="45">
+        <v>7000.7</v>
+      </c>
+      <c r="F35" s="45">
+        <v>7000.7</v>
+      </c>
+      <c r="G35" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="36" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C36" s="38"/>
+      <c r="D36" s="38"/>
+      <c r="E36" s="37"/>
+      <c r="F36" s="37"/>
+    </row>
+    <row r="37" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B37" s="38" t="s">
+        <v>328</v>
+      </c>
+      <c r="D37" s="38"/>
+      <c r="E37" s="37"/>
+      <c r="F37" s="37"/>
+    </row>
+    <row r="38" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C38" s="38" t="s">
+        <v>329</v>
+      </c>
+      <c r="D38" s="38"/>
+      <c r="E38" s="46">
+        <v>7000.8</v>
+      </c>
+      <c r="F38" s="45">
+        <v>7000.8</v>
+      </c>
+      <c r="G38" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="39" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C39" s="38" t="s">
+        <v>331</v>
+      </c>
+      <c r="D39" s="38"/>
+      <c r="E39" s="44">
+        <v>7000.9</v>
+      </c>
+      <c r="F39" s="44">
+        <v>7000.9</v>
+      </c>
+      <c r="G39" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="40" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C40" s="38"/>
+      <c r="D40" s="38"/>
+      <c r="E40" s="37"/>
+      <c r="F40" s="37"/>
+    </row>
+    <row r="41" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B41" s="38" t="s">
+        <v>333</v>
+      </c>
+      <c r="D41" s="38"/>
+      <c r="E41" s="36"/>
+      <c r="F41" s="36"/>
+      <c r="G41" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="42" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C42" s="38"/>
+      <c r="D42" s="38"/>
+      <c r="E42" s="37"/>
+      <c r="F42" s="37"/>
+    </row>
+    <row r="43" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B43" s="38" t="s">
+        <v>335</v>
+      </c>
+      <c r="D43" s="38"/>
+      <c r="E43" s="37"/>
+      <c r="F43" s="37"/>
+    </row>
+    <row r="44" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C44" s="38" t="s">
+        <v>336</v>
+      </c>
+      <c r="D44" s="38"/>
+      <c r="E44" s="36"/>
+      <c r="F44" s="36"/>
+      <c r="G44" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="45" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C45" s="38" t="s">
+        <v>322</v>
+      </c>
+      <c r="D45" s="38"/>
+      <c r="E45" s="44">
+        <v>7400.2</v>
+      </c>
+      <c r="F45" s="44">
+        <v>7400.2</v>
+      </c>
+      <c r="G45" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="46" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C46" s="38"/>
+      <c r="D46" s="38"/>
+      <c r="E46" s="37"/>
+      <c r="F46" s="37"/>
+    </row>
+    <row r="47" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B47" s="38" t="s">
+        <v>339</v>
+      </c>
+      <c r="D47" s="38"/>
+      <c r="E47" s="45">
+        <v>7400.1</v>
+      </c>
+      <c r="F47" s="45">
+        <v>7400.1</v>
+      </c>
+      <c r="G47" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="48" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C48" s="38"/>
+      <c r="D48" s="38"/>
+      <c r="E48" s="37"/>
+      <c r="F48" s="37"/>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B49" s="38" t="s">
+        <v>341</v>
+      </c>
+      <c r="D49" s="38"/>
+      <c r="E49" s="47" t="s">
+        <v>342</v>
+      </c>
+      <c r="F49" s="47" t="s">
+        <v>342</v>
+      </c>
+      <c r="G49" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C50" s="48"/>
+      <c r="D50" s="38"/>
+      <c r="E50" s="36"/>
+      <c r="F50" s="36"/>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C51" s="49"/>
+      <c r="D51" s="38"/>
+      <c r="E51" s="42"/>
+      <c r="F51" s="42"/>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C52" s="49"/>
+      <c r="D52" s="38"/>
+      <c r="E52" s="42"/>
+      <c r="F52" s="42"/>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C53" s="49"/>
+      <c r="D53" s="38"/>
+      <c r="E53" s="42"/>
+      <c r="F53" s="42"/>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C54" s="49"/>
+      <c r="D54" s="38"/>
+      <c r="E54" s="42"/>
+      <c r="F54" s="42"/>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C55" s="49"/>
+      <c r="D55" s="38"/>
+      <c r="E55" s="42"/>
+      <c r="F55" s="42"/>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C56" s="38"/>
+      <c r="D56" s="38"/>
+      <c r="E56" s="37"/>
+      <c r="F56" s="37"/>
+    </row>
+    <row r="57" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A57" s="50" t="s">
+        <v>344</v>
+      </c>
+      <c r="D57" s="50"/>
+      <c r="E57" s="51"/>
+      <c r="F57" s="51"/>
+      <c r="G57" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A59" s="32" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B60" s="34" t="s">
+        <v>347</v>
+      </c>
+      <c r="D60" s="34"/>
+      <c r="E60" s="36"/>
+      <c r="F60" s="36"/>
+      <c r="G60" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B61" s="34"/>
+      <c r="D61" s="34"/>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B62" s="34" t="s">
+        <v>349</v>
+      </c>
+      <c r="D62" s="34"/>
+      <c r="E62" s="45"/>
+      <c r="F62" s="45"/>
+      <c r="G62" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B63" s="34"/>
+      <c r="D63" s="34"/>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B64" s="34" t="s">
+        <v>351</v>
+      </c>
+      <c r="D64" s="34"/>
+      <c r="E64" s="36"/>
+      <c r="F64" s="36"/>
+      <c r="G64" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="65" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C65" s="34"/>
+      <c r="D65" s="34"/>
+    </row>
+    <row r="66" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B66" s="34" t="s">
+        <v>353</v>
+      </c>
+      <c r="D66" s="34"/>
+    </row>
+    <row r="67" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C67" s="34" t="s">
+        <v>354</v>
+      </c>
+      <c r="D67" s="34"/>
+      <c r="E67" s="36"/>
+      <c r="F67" s="36"/>
+      <c r="G67" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="68" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C68" s="34" t="s">
+        <v>356</v>
+      </c>
+      <c r="D68" s="34"/>
+      <c r="E68" s="36"/>
+      <c r="F68" s="36"/>
+      <c r="G68" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="69" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C69" s="34" t="s">
+        <v>358</v>
+      </c>
+      <c r="D69" s="34"/>
+      <c r="E69" s="36"/>
+      <c r="F69" s="36"/>
+      <c r="G69" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="70" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C70" s="34"/>
+      <c r="D70" s="34"/>
+    </row>
+    <row r="71" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B71" s="34" t="s">
+        <v>360</v>
+      </c>
+      <c r="D71" s="34"/>
+    </row>
+    <row r="72" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C72" s="34" t="s">
+        <v>361</v>
+      </c>
+      <c r="D72" s="34"/>
+      <c r="E72" s="36"/>
+      <c r="F72" s="36"/>
+      <c r="G72" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="73" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C73" s="34" t="s">
+        <v>363</v>
+      </c>
+      <c r="D73" s="34"/>
+      <c r="E73" s="36"/>
+      <c r="F73" s="36"/>
+      <c r="G73" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="74" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C74" s="34"/>
+      <c r="D74" s="34"/>
+    </row>
+    <row r="75" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B75" s="34" t="s">
+        <v>365</v>
+      </c>
+      <c r="D75" s="34"/>
+      <c r="E75" s="45">
+        <v>7420</v>
+      </c>
+      <c r="F75" s="45">
+        <v>7420</v>
+      </c>
+      <c r="G75" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="76" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C76" s="34"/>
+      <c r="D76" s="34"/>
+    </row>
+    <row r="77" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B77" s="34" t="s">
+        <v>367</v>
+      </c>
+      <c r="D77" s="34"/>
+      <c r="E77" s="36"/>
+      <c r="F77" s="36"/>
+      <c r="G77" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="78" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B78" s="34"/>
+      <c r="D78" s="34"/>
+    </row>
+    <row r="79" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B79" s="34" t="s">
+        <v>369</v>
+      </c>
+      <c r="D79" s="34"/>
+      <c r="E79" s="36"/>
+      <c r="F79" s="36"/>
+      <c r="G79" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="80" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B80" s="34"/>
+      <c r="D80" s="34"/>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B81" s="34" t="s">
+        <v>371</v>
+      </c>
+      <c r="D81" s="34"/>
+      <c r="E81" s="36"/>
+      <c r="F81" s="36"/>
+      <c r="G81" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B82" s="34"/>
+      <c r="D82" s="34"/>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B83" s="34" t="s">
+        <v>373</v>
+      </c>
+      <c r="D83" s="34"/>
+      <c r="E83" s="36"/>
+      <c r="F83" s="36"/>
+      <c r="G83" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C84" s="48"/>
+      <c r="D84" s="38"/>
+      <c r="E84" s="36"/>
+      <c r="F84" s="36"/>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C85" s="48"/>
+      <c r="D85" s="38"/>
+      <c r="E85" s="36"/>
+      <c r="F85" s="36"/>
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C86" s="48"/>
+      <c r="D86" s="38"/>
+      <c r="E86" s="36"/>
+      <c r="F86" s="36"/>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C87" s="48"/>
+      <c r="D87" s="38"/>
+      <c r="E87" s="36"/>
+      <c r="F87" s="36"/>
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C88" s="48"/>
+      <c r="D88" s="38"/>
+      <c r="E88" s="36"/>
+      <c r="F88" s="36"/>
+    </row>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C89" s="48"/>
+      <c r="D89" s="38"/>
+      <c r="E89" s="36"/>
+      <c r="F89" s="36"/>
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C90" s="48"/>
+      <c r="D90" s="38"/>
+      <c r="E90" s="36"/>
+      <c r="F90" s="36"/>
+    </row>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C91" s="38"/>
+      <c r="D91" s="38"/>
+      <c r="E91" s="37"/>
+      <c r="F91" s="37"/>
+    </row>
+    <row r="92" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A92" s="52" t="s">
+        <v>375</v>
+      </c>
+      <c r="D92" s="52"/>
+      <c r="E92" s="53"/>
+      <c r="F92" s="53"/>
+      <c r="G92" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="C93" s="34"/>
+      <c r="D93" s="34"/>
+    </row>
+    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A94" s="34" t="s">
+        <v>377</v>
+      </c>
+      <c r="D94" s="34"/>
+      <c r="E94" s="36"/>
+      <c r="F94" s="36"/>
+      <c r="G94" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A95" s="34" t="s">
+        <v>379</v>
+      </c>
+      <c r="D95" s="34"/>
+      <c r="E95" s="44">
+        <v>7500</v>
+      </c>
+      <c r="F95" s="44">
+        <v>7500</v>
+      </c>
+      <c r="G95" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A96" s="34" t="s">
+        <v>381</v>
+      </c>
+      <c r="D96" s="34"/>
+      <c r="E96" s="42"/>
+      <c r="F96" s="42"/>
+      <c r="G96" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A97" s="34" t="s">
+        <v>383</v>
+      </c>
+      <c r="D97" s="34"/>
+      <c r="E97" s="42"/>
+      <c r="F97" s="42"/>
+      <c r="G97" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A98" s="34" t="s">
+        <v>385</v>
+      </c>
+      <c r="D98" s="34"/>
+      <c r="E98" s="53"/>
+      <c r="F98" s="53"/>
+      <c r="G98" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
   <customProperties>
-    <customPr name="OrphanNamesChecked" r:id="rId1"/>
+    <customPr name="OrphanNamesChecked" r:id="rId2"/>
   </customProperties>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.140625" customWidth="1"/>
+    <col min="3" max="3" width="20.140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="8.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>117</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
     </row>
   </sheetData>
@@ -4077,11 +5274,50 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="24" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <customProperties>
+    <customPr name="OrphanNamesChecked" r:id="rId1"/>
+  </customProperties>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <customProperties>

</xml_diff>

<commit_message>
enhanced form1 output formatter -> cleaner and fixed bugs on error when opening file
</commit_message>
<xml_diff>
--- a/parameters/mas_forms_tb_mapping.xlsx
+++ b/parameters/mas_forms_tb_mapping.xlsx
@@ -4,13 +4,13 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6315" firstSheet="1" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6315" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="Agreed options" sheetId="4" state="hidden" r:id="rId1"/>
-    <sheet name="Form 1 - TB mapping" sheetId="17" r:id="rId2"/>
-    <sheet name="Form 1 - Qns for user inputs" sheetId="18" r:id="rId3"/>
-    <sheet name="Form 3 - TB mapping" sheetId="19" r:id="rId4"/>
+    <sheet name="Form 1 - TB mapping" sheetId="17" r:id="rId1"/>
+    <sheet name="Form 1 - Qns for user inputs" sheetId="18" r:id="rId2"/>
+    <sheet name="Form 3 - TB mapping" sheetId="19" r:id="rId3"/>
+    <sheet name="Agreed options" sheetId="4" state="hidden" r:id="rId4"/>
     <sheet name="AR AP listing template" sheetId="10" state="hidden" r:id="rId5"/>
     <sheet name="AR AP ageing template" sheetId="11" state="hidden" r:id="rId6"/>
     <sheet name="RPT template" sheetId="12" state="hidden" r:id="rId7"/>
@@ -1649,27 +1649,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1720,6 +1699,27 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2007,43 +2007,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:A3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>99</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <customProperties>
-    <customPr name="OrphanNamesChecked" r:id="rId1"/>
-  </customProperties>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H238"/>
   <sheetViews>
-    <sheetView topLeftCell="A151" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="H176" activeCellId="1" sqref="H173:H174 H176"/>
     </sheetView>
   </sheetViews>
@@ -2067,10 +2034,10 @@
       <c r="E1" s="2"/>
     </row>
     <row r="2" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="47" t="s">
         <v>101</v>
       </c>
-      <c r="B2" s="26"/>
+      <c r="B2" s="48"/>
       <c r="C2" s="11" t="s">
         <v>251</v>
       </c>
@@ -2078,10 +2045,10 @@
       <c r="E2" s="3"/>
     </row>
     <row r="3" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="27" t="s">
+      <c r="A3" s="49" t="s">
         <v>102</v>
       </c>
-      <c r="B3" s="28"/>
+      <c r="B3" s="50"/>
       <c r="C3" s="12" t="s">
         <v>112</v>
       </c>
@@ -2089,10 +2056,10 @@
       <c r="E3" s="4"/>
     </row>
     <row r="4" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="27" t="s">
+      <c r="A4" s="49" t="s">
         <v>103</v>
       </c>
-      <c r="B4" s="28"/>
+      <c r="B4" s="50"/>
       <c r="C4" s="12" t="s">
         <v>111</v>
       </c>
@@ -2100,10 +2067,10 @@
       <c r="E4" s="4"/>
     </row>
     <row r="5" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="29" t="s">
+      <c r="A5" s="51" t="s">
         <v>104</v>
       </c>
-      <c r="B5" s="30"/>
+      <c r="B5" s="52"/>
       <c r="C5" s="13"/>
       <c r="D5" s="5"/>
       <c r="E5" s="5"/>
@@ -2254,10 +2221,10 @@
       <c r="G21" s="19"/>
     </row>
     <row r="22" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A22" s="31" t="s">
+      <c r="A22" s="53" t="s">
         <v>7</v>
       </c>
-      <c r="B22" s="31"/>
+      <c r="B22" s="53"/>
       <c r="C22" s="8"/>
       <c r="D22" s="8"/>
       <c r="E22" s="8"/>
@@ -4252,7 +4219,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C12"/>
   <sheetViews>
@@ -4384,29 +4351,29 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A4:G99"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="82" workbookViewId="0">
-      <selection activeCell="D54" sqref="D54"/>
+    <sheetView tabSelected="1" zoomScale="82" workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="32"/>
-    <col min="2" max="2" width="4.85546875" style="32" customWidth="1"/>
-    <col min="3" max="3" width="8.42578125" style="32" customWidth="1"/>
-    <col min="4" max="4" width="86.5703125" style="32" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="25"/>
+    <col min="2" max="2" width="4.85546875" style="25" customWidth="1"/>
+    <col min="3" max="3" width="8.42578125" style="25" customWidth="1"/>
+    <col min="4" max="4" width="86.5703125" style="25" customWidth="1"/>
     <col min="5" max="5" width="21" customWidth="1"/>
     <col min="6" max="6" width="21.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="4" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="E4" s="33" t="s">
+      <c r="E4" s="26" t="s">
         <v>284</v>
       </c>
-      <c r="F4" s="33" t="s">
+      <c r="F4" s="26" t="s">
         <v>285</v>
       </c>
       <c r="G4" t="s">
@@ -4414,192 +4381,192 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="32" t="s">
+      <c r="A5" s="25" t="s">
         <v>287</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B6" s="34" t="s">
+      <c r="B6" s="27" t="s">
         <v>288</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C7" s="34" t="s">
+      <c r="C7" s="27" t="s">
         <v>289</v>
       </c>
-      <c r="D7" s="34"/>
+      <c r="D7" s="27"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D8" s="35" t="s">
+      <c r="D8" s="28" t="s">
         <v>290</v>
       </c>
-      <c r="E8" s="36"/>
-      <c r="F8" s="36"/>
+      <c r="E8" s="29"/>
+      <c r="F8" s="29"/>
       <c r="G8" t="s">
         <v>291</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D9" s="35" t="s">
+      <c r="D9" s="28" t="s">
         <v>292</v>
       </c>
-      <c r="E9" s="36"/>
-      <c r="F9" s="36"/>
+      <c r="E9" s="29"/>
+      <c r="F9" s="29"/>
       <c r="G9" t="s">
         <v>293</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C10" s="35"/>
-      <c r="D10" s="35"/>
-      <c r="E10" s="37"/>
-      <c r="F10" s="37"/>
+      <c r="C10" s="28"/>
+      <c r="D10" s="28"/>
+      <c r="E10" s="30"/>
+      <c r="F10" s="30"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C11" s="38" t="s">
+      <c r="C11" s="31" t="s">
         <v>294</v>
       </c>
-      <c r="D11" s="38"/>
+      <c r="D11" s="31"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D12" s="39" t="s">
+      <c r="D12" s="32" t="s">
         <v>290</v>
       </c>
-      <c r="E12" s="36"/>
-      <c r="F12" s="36"/>
+      <c r="E12" s="29"/>
+      <c r="F12" s="29"/>
       <c r="G12" t="s">
         <v>295</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="D13" s="39" t="s">
+      <c r="D13" s="32" t="s">
         <v>296</v>
       </c>
-      <c r="E13" s="36"/>
-      <c r="F13" s="36"/>
+      <c r="E13" s="29"/>
+      <c r="F13" s="29"/>
       <c r="G13" t="s">
         <v>297</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="D14" s="39" t="s">
+      <c r="D14" s="32" t="s">
         <v>298</v>
       </c>
-      <c r="E14" s="36"/>
-      <c r="F14" s="36"/>
+      <c r="E14" s="29"/>
+      <c r="F14" s="29"/>
       <c r="G14" t="s">
         <v>299</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C15" s="40"/>
-      <c r="D15" s="40"/>
-      <c r="E15" s="37"/>
-      <c r="F15" s="37"/>
+      <c r="C15" s="33"/>
+      <c r="D15" s="33"/>
+      <c r="E15" s="30"/>
+      <c r="F15" s="30"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B16" s="41" t="s">
+      <c r="B16" s="34" t="s">
         <v>300</v>
       </c>
-      <c r="D16" s="41"/>
+      <c r="D16" s="34"/>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C17" s="40" t="s">
+      <c r="C17" s="33" t="s">
         <v>301</v>
       </c>
-      <c r="D17" s="40"/>
-      <c r="E17" s="36"/>
-      <c r="F17" s="36"/>
+      <c r="D17" s="33"/>
+      <c r="E17" s="29"/>
+      <c r="F17" s="29"/>
       <c r="G17" t="s">
         <v>302</v>
       </c>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C18" s="40" t="s">
+      <c r="C18" s="33" t="s">
         <v>303</v>
       </c>
-      <c r="D18" s="40"/>
-      <c r="E18" s="42"/>
-      <c r="F18" s="42"/>
+      <c r="D18" s="33"/>
+      <c r="E18" s="35"/>
+      <c r="F18" s="35"/>
       <c r="G18" t="s">
         <v>304</v>
       </c>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C19" s="40" t="s">
+      <c r="C19" s="33" t="s">
         <v>305</v>
       </c>
-      <c r="D19" s="40"/>
-      <c r="E19" s="42"/>
-      <c r="F19" s="42"/>
+      <c r="D19" s="33"/>
+      <c r="E19" s="35"/>
+      <c r="F19" s="35"/>
       <c r="G19" t="s">
         <v>306</v>
       </c>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C20" s="40" t="s">
+      <c r="C20" s="33" t="s">
         <v>307</v>
       </c>
-      <c r="D20" s="40"/>
-      <c r="E20" s="42"/>
-      <c r="F20" s="42"/>
+      <c r="D20" s="33"/>
+      <c r="E20" s="35"/>
+      <c r="F20" s="35"/>
       <c r="G20" t="s">
         <v>308</v>
       </c>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C21" s="38" t="s">
+      <c r="C21" s="31" t="s">
         <v>309</v>
       </c>
-      <c r="D21" s="38"/>
-      <c r="E21" s="42"/>
-      <c r="F21" s="42"/>
+      <c r="D21" s="31"/>
+      <c r="E21" s="35"/>
+      <c r="F21" s="35"/>
       <c r="G21" t="s">
         <v>310</v>
       </c>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C22" s="38"/>
-      <c r="D22" s="38" t="s">
+      <c r="C22" s="31"/>
+      <c r="D22" s="31" t="s">
         <v>311</v>
       </c>
-      <c r="E22" s="37"/>
-      <c r="F22" s="37"/>
+      <c r="E22" s="30"/>
+      <c r="F22" s="30"/>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B23" s="38" t="s">
+      <c r="B23" s="31" t="s">
         <v>312</v>
       </c>
-      <c r="D23" s="38"/>
-      <c r="E23" s="36"/>
-      <c r="F23" s="36"/>
+      <c r="D23" s="31"/>
+      <c r="E23" s="29"/>
+      <c r="F23" s="29"/>
       <c r="G23" t="s">
         <v>313</v>
       </c>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C24" s="38"/>
-      <c r="D24" s="38"/>
-      <c r="E24" s="37"/>
-      <c r="F24" s="37"/>
+      <c r="C24" s="31"/>
+      <c r="D24" s="31"/>
+      <c r="E24" s="30"/>
+      <c r="F24" s="30"/>
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B25" s="38" t="s">
+      <c r="B25" s="31" t="s">
         <v>314</v>
       </c>
-      <c r="D25" s="38"/>
-      <c r="E25" s="37"/>
-      <c r="F25" s="37"/>
+      <c r="D25" s="31"/>
+      <c r="E25" s="30"/>
+      <c r="F25" s="30"/>
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C26" s="38" t="s">
+      <c r="C26" s="31" t="s">
         <v>315</v>
       </c>
-      <c r="D26" s="38"/>
-      <c r="E26" s="43">
+      <c r="D26" s="31"/>
+      <c r="E26" s="36">
         <v>7000.1</v>
       </c>
-      <c r="F26" s="43">
+      <c r="F26" s="36">
         <v>7000.1</v>
       </c>
       <c r="G26" t="s">
@@ -4607,14 +4574,14 @@
       </c>
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C27" s="38" t="s">
+      <c r="C27" s="31" t="s">
         <v>317</v>
       </c>
-      <c r="D27" s="38"/>
-      <c r="E27" s="44">
+      <c r="D27" s="31"/>
+      <c r="E27" s="37">
         <v>7000.2</v>
       </c>
-      <c r="F27" s="44">
+      <c r="F27" s="37">
         <v>7000.2</v>
       </c>
       <c r="G27" t="s">
@@ -4622,28 +4589,28 @@
       </c>
     </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C28" s="38"/>
-      <c r="D28" s="38"/>
-      <c r="E28" s="37"/>
-      <c r="F28" s="37"/>
+      <c r="C28" s="31"/>
+      <c r="D28" s="31"/>
+      <c r="E28" s="30"/>
+      <c r="F28" s="30"/>
     </row>
     <row r="29" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B29" s="38" t="s">
+      <c r="B29" s="31" t="s">
         <v>319</v>
       </c>
-      <c r="D29" s="38"/>
-      <c r="E29" s="37"/>
-      <c r="F29" s="37"/>
+      <c r="D29" s="31"/>
+      <c r="E29" s="30"/>
+      <c r="F29" s="30"/>
     </row>
     <row r="30" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C30" s="38" t="s">
+      <c r="C30" s="31" t="s">
         <v>320</v>
       </c>
-      <c r="D30" s="38"/>
-      <c r="E30" s="45">
+      <c r="D30" s="31"/>
+      <c r="E30" s="38">
         <v>7000.4</v>
       </c>
-      <c r="F30" s="45">
+      <c r="F30" s="38">
         <v>7000.4</v>
       </c>
       <c r="G30" t="s">
@@ -4651,14 +4618,14 @@
       </c>
     </row>
     <row r="31" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C31" s="38" t="s">
+      <c r="C31" s="31" t="s">
         <v>322</v>
       </c>
-      <c r="D31" s="38"/>
-      <c r="E31" s="44">
+      <c r="D31" s="31"/>
+      <c r="E31" s="37">
         <v>7000.5</v>
       </c>
-      <c r="F31" s="44">
+      <c r="F31" s="37">
         <v>7000.5</v>
       </c>
       <c r="G31" t="s">
@@ -4666,20 +4633,20 @@
       </c>
     </row>
     <row r="32" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C32" s="38"/>
-      <c r="D32" s="38"/>
-      <c r="E32" s="37"/>
-      <c r="F32" s="37"/>
+      <c r="C32" s="31"/>
+      <c r="D32" s="31"/>
+      <c r="E32" s="30"/>
+      <c r="F32" s="30"/>
     </row>
     <row r="33" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B33" s="38" t="s">
+      <c r="B33" s="31" t="s">
         <v>324</v>
       </c>
-      <c r="D33" s="38"/>
-      <c r="E33" s="45">
+      <c r="D33" s="31"/>
+      <c r="E33" s="38">
         <v>7000.6</v>
       </c>
-      <c r="F33" s="45">
+      <c r="F33" s="38">
         <v>7000.6</v>
       </c>
       <c r="G33" t="s">
@@ -4687,20 +4654,20 @@
       </c>
     </row>
     <row r="34" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C34" s="38"/>
-      <c r="D34" s="38"/>
-      <c r="E34" s="37"/>
-      <c r="F34" s="37"/>
+      <c r="C34" s="31"/>
+      <c r="D34" s="31"/>
+      <c r="E34" s="30"/>
+      <c r="F34" s="30"/>
     </row>
     <row r="35" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B35" s="38" t="s">
+      <c r="B35" s="31" t="s">
         <v>326</v>
       </c>
-      <c r="D35" s="38"/>
-      <c r="E35" s="45">
+      <c r="D35" s="31"/>
+      <c r="E35" s="38">
         <v>7000.7</v>
       </c>
-      <c r="F35" s="45">
+      <c r="F35" s="38">
         <v>7000.7</v>
       </c>
       <c r="G35" t="s">
@@ -4708,28 +4675,28 @@
       </c>
     </row>
     <row r="36" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C36" s="38"/>
-      <c r="D36" s="38"/>
-      <c r="E36" s="37"/>
-      <c r="F36" s="37"/>
+      <c r="C36" s="31"/>
+      <c r="D36" s="31"/>
+      <c r="E36" s="30"/>
+      <c r="F36" s="30"/>
     </row>
     <row r="37" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B37" s="38" t="s">
+      <c r="B37" s="31" t="s">
         <v>328</v>
       </c>
-      <c r="D37" s="38"/>
-      <c r="E37" s="37"/>
-      <c r="F37" s="37"/>
+      <c r="D37" s="31"/>
+      <c r="E37" s="30"/>
+      <c r="F37" s="30"/>
     </row>
     <row r="38" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C38" s="38" t="s">
+      <c r="C38" s="31" t="s">
         <v>329</v>
       </c>
-      <c r="D38" s="38"/>
-      <c r="E38" s="46">
+      <c r="D38" s="31"/>
+      <c r="E38" s="39">
         <v>7000.8</v>
       </c>
-      <c r="F38" s="45">
+      <c r="F38" s="38">
         <v>7000.8</v>
       </c>
       <c r="G38" t="s">
@@ -4737,14 +4704,14 @@
       </c>
     </row>
     <row r="39" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C39" s="38" t="s">
+      <c r="C39" s="31" t="s">
         <v>331</v>
       </c>
-      <c r="D39" s="38"/>
-      <c r="E39" s="44">
+      <c r="D39" s="31"/>
+      <c r="E39" s="37">
         <v>7000.9</v>
       </c>
-      <c r="F39" s="44">
+      <c r="F39" s="37">
         <v>7000.9</v>
       </c>
       <c r="G39" t="s">
@@ -4752,56 +4719,56 @@
       </c>
     </row>
     <row r="40" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C40" s="38"/>
-      <c r="D40" s="38"/>
-      <c r="E40" s="37"/>
-      <c r="F40" s="37"/>
+      <c r="C40" s="31"/>
+      <c r="D40" s="31"/>
+      <c r="E40" s="30"/>
+      <c r="F40" s="30"/>
     </row>
     <row r="41" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B41" s="38" t="s">
+      <c r="B41" s="31" t="s">
         <v>333</v>
       </c>
-      <c r="D41" s="38"/>
-      <c r="E41" s="36"/>
-      <c r="F41" s="36"/>
+      <c r="D41" s="31"/>
+      <c r="E41" s="29"/>
+      <c r="F41" s="29"/>
       <c r="G41" t="s">
         <v>334</v>
       </c>
     </row>
     <row r="42" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C42" s="38"/>
-      <c r="D42" s="38"/>
-      <c r="E42" s="37"/>
-      <c r="F42" s="37"/>
+      <c r="C42" s="31"/>
+      <c r="D42" s="31"/>
+      <c r="E42" s="30"/>
+      <c r="F42" s="30"/>
     </row>
     <row r="43" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B43" s="38" t="s">
+      <c r="B43" s="31" t="s">
         <v>335</v>
       </c>
-      <c r="D43" s="38"/>
-      <c r="E43" s="37"/>
-      <c r="F43" s="37"/>
+      <c r="D43" s="31"/>
+      <c r="E43" s="30"/>
+      <c r="F43" s="30"/>
     </row>
     <row r="44" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C44" s="38" t="s">
+      <c r="C44" s="31" t="s">
         <v>336</v>
       </c>
-      <c r="D44" s="38"/>
-      <c r="E44" s="36"/>
-      <c r="F44" s="36"/>
+      <c r="D44" s="31"/>
+      <c r="E44" s="29"/>
+      <c r="F44" s="29"/>
       <c r="G44" t="s">
         <v>337</v>
       </c>
     </row>
     <row r="45" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C45" s="38" t="s">
+      <c r="C45" s="31" t="s">
         <v>322</v>
       </c>
-      <c r="D45" s="38"/>
-      <c r="E45" s="44">
+      <c r="D45" s="31"/>
+      <c r="E45" s="37">
         <v>7400.2</v>
       </c>
-      <c r="F45" s="44">
+      <c r="F45" s="37">
         <v>7400.2</v>
       </c>
       <c r="G45" t="s">
@@ -4809,20 +4776,20 @@
       </c>
     </row>
     <row r="46" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C46" s="38"/>
-      <c r="D46" s="38"/>
-      <c r="E46" s="37"/>
-      <c r="F46" s="37"/>
+      <c r="C46" s="31"/>
+      <c r="D46" s="31"/>
+      <c r="E46" s="30"/>
+      <c r="F46" s="30"/>
     </row>
     <row r="47" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B47" s="38" t="s">
+      <c r="B47" s="31" t="s">
         <v>339</v>
       </c>
-      <c r="D47" s="38"/>
-      <c r="E47" s="45">
+      <c r="D47" s="31"/>
+      <c r="E47" s="38">
         <v>7400.1</v>
       </c>
-      <c r="F47" s="45">
+      <c r="F47" s="38">
         <v>7400.1</v>
       </c>
       <c r="G47" t="s">
@@ -4830,20 +4797,20 @@
       </c>
     </row>
     <row r="48" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C48" s="38"/>
-      <c r="D48" s="38"/>
-      <c r="E48" s="37"/>
-      <c r="F48" s="37"/>
+      <c r="C48" s="31"/>
+      <c r="D48" s="31"/>
+      <c r="E48" s="30"/>
+      <c r="F48" s="30"/>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B49" s="38" t="s">
+      <c r="B49" s="31" t="s">
         <v>341</v>
       </c>
-      <c r="D49" s="38"/>
-      <c r="E49" s="47" t="s">
+      <c r="D49" s="31"/>
+      <c r="E49" s="40" t="s">
         <v>342</v>
       </c>
-      <c r="F49" s="47" t="s">
+      <c r="F49" s="40" t="s">
         <v>342</v>
       </c>
       <c r="G49" t="s">
@@ -4851,193 +4818,193 @@
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C50" s="48"/>
-      <c r="D50" s="38"/>
-      <c r="E50" s="36"/>
-      <c r="F50" s="36"/>
+      <c r="C50" s="41"/>
+      <c r="D50" s="31"/>
+      <c r="E50" s="29"/>
+      <c r="F50" s="29"/>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C51" s="49"/>
-      <c r="D51" s="38"/>
-      <c r="E51" s="42"/>
-      <c r="F51" s="42"/>
+      <c r="C51" s="42"/>
+      <c r="D51" s="31"/>
+      <c r="E51" s="35"/>
+      <c r="F51" s="35"/>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C52" s="49"/>
-      <c r="D52" s="38"/>
-      <c r="E52" s="42"/>
-      <c r="F52" s="42"/>
+      <c r="C52" s="42"/>
+      <c r="D52" s="31"/>
+      <c r="E52" s="35"/>
+      <c r="F52" s="35"/>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C53" s="49"/>
-      <c r="D53" s="38"/>
-      <c r="E53" s="42"/>
-      <c r="F53" s="42"/>
+      <c r="C53" s="42"/>
+      <c r="D53" s="31"/>
+      <c r="E53" s="35"/>
+      <c r="F53" s="35"/>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C54" s="49"/>
-      <c r="D54" s="38"/>
-      <c r="E54" s="42"/>
-      <c r="F54" s="42"/>
+      <c r="C54" s="42"/>
+      <c r="D54" s="31"/>
+      <c r="E54" s="35"/>
+      <c r="F54" s="35"/>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C55" s="49"/>
-      <c r="D55" s="38"/>
-      <c r="E55" s="42"/>
-      <c r="F55" s="42"/>
+      <c r="C55" s="42"/>
+      <c r="D55" s="31"/>
+      <c r="E55" s="35"/>
+      <c r="F55" s="35"/>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C56" s="38"/>
-      <c r="D56" s="38"/>
-      <c r="E56" s="37"/>
-      <c r="F56" s="37"/>
+      <c r="C56" s="31"/>
+      <c r="D56" s="31"/>
+      <c r="E56" s="30"/>
+      <c r="F56" s="30"/>
     </row>
     <row r="57" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="50" t="s">
+      <c r="A57" s="43" t="s">
         <v>344</v>
       </c>
-      <c r="D57" s="50"/>
-      <c r="E57" s="51"/>
-      <c r="F57" s="51"/>
+      <c r="D57" s="43"/>
+      <c r="E57" s="44"/>
+      <c r="F57" s="44"/>
       <c r="G57" t="s">
         <v>345</v>
       </c>
     </row>
     <row r="58" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A59" s="32" t="s">
+      <c r="A59" s="25" t="s">
         <v>346</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B60" s="34" t="s">
+      <c r="B60" s="27" t="s">
         <v>347</v>
       </c>
-      <c r="D60" s="34"/>
-      <c r="E60" s="36"/>
-      <c r="F60" s="36"/>
+      <c r="D60" s="27"/>
+      <c r="E60" s="29"/>
+      <c r="F60" s="29"/>
       <c r="G60" t="s">
         <v>348</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B61" s="34"/>
-      <c r="D61" s="34"/>
+      <c r="B61" s="27"/>
+      <c r="D61" s="27"/>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B62" s="34" t="s">
+      <c r="B62" s="27" t="s">
         <v>349</v>
       </c>
-      <c r="D62" s="34"/>
-      <c r="E62" s="45"/>
-      <c r="F62" s="45"/>
+      <c r="D62" s="27"/>
+      <c r="E62" s="38"/>
+      <c r="F62" s="38"/>
       <c r="G62" t="s">
         <v>350</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B63" s="34"/>
-      <c r="D63" s="34"/>
+      <c r="B63" s="27"/>
+      <c r="D63" s="27"/>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B64" s="34" t="s">
+      <c r="B64" s="27" t="s">
         <v>351</v>
       </c>
-      <c r="D64" s="34"/>
-      <c r="E64" s="36"/>
-      <c r="F64" s="36"/>
+      <c r="D64" s="27"/>
+      <c r="E64" s="29"/>
+      <c r="F64" s="29"/>
       <c r="G64" t="s">
         <v>352</v>
       </c>
     </row>
     <row r="65" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C65" s="34"/>
-      <c r="D65" s="34"/>
+      <c r="C65" s="27"/>
+      <c r="D65" s="27"/>
     </row>
     <row r="66" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B66" s="34" t="s">
+      <c r="B66" s="27" t="s">
         <v>353</v>
       </c>
-      <c r="D66" s="34"/>
+      <c r="D66" s="27"/>
     </row>
     <row r="67" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C67" s="34" t="s">
+      <c r="C67" s="27" t="s">
         <v>354</v>
       </c>
-      <c r="D67" s="34"/>
-      <c r="E67" s="36"/>
-      <c r="F67" s="36"/>
+      <c r="D67" s="27"/>
+      <c r="E67" s="29"/>
+      <c r="F67" s="29"/>
       <c r="G67" t="s">
         <v>355</v>
       </c>
     </row>
     <row r="68" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C68" s="34" t="s">
+      <c r="C68" s="27" t="s">
         <v>356</v>
       </c>
-      <c r="D68" s="34"/>
-      <c r="E68" s="36"/>
-      <c r="F68" s="36"/>
+      <c r="D68" s="27"/>
+      <c r="E68" s="29"/>
+      <c r="F68" s="29"/>
       <c r="G68" t="s">
         <v>357</v>
       </c>
     </row>
     <row r="69" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C69" s="34" t="s">
+      <c r="C69" s="27" t="s">
         <v>358</v>
       </c>
-      <c r="D69" s="34"/>
-      <c r="E69" s="36"/>
-      <c r="F69" s="36"/>
+      <c r="D69" s="27"/>
+      <c r="E69" s="29"/>
+      <c r="F69" s="29"/>
       <c r="G69" t="s">
         <v>359</v>
       </c>
     </row>
     <row r="70" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C70" s="34"/>
-      <c r="D70" s="34"/>
+      <c r="C70" s="27"/>
+      <c r="D70" s="27"/>
     </row>
     <row r="71" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B71" s="34" t="s">
+      <c r="B71" s="27" t="s">
         <v>360</v>
       </c>
-      <c r="D71" s="34"/>
+      <c r="D71" s="27"/>
     </row>
     <row r="72" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C72" s="34" t="s">
+      <c r="C72" s="27" t="s">
         <v>361</v>
       </c>
-      <c r="D72" s="34"/>
-      <c r="E72" s="36"/>
-      <c r="F72" s="36"/>
+      <c r="D72" s="27"/>
+      <c r="E72" s="29"/>
+      <c r="F72" s="29"/>
       <c r="G72" t="s">
         <v>362</v>
       </c>
     </row>
     <row r="73" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C73" s="34" t="s">
+      <c r="C73" s="27" t="s">
         <v>363</v>
       </c>
-      <c r="D73" s="34"/>
-      <c r="E73" s="36"/>
-      <c r="F73" s="36"/>
+      <c r="D73" s="27"/>
+      <c r="E73" s="29"/>
+      <c r="F73" s="29"/>
       <c r="G73" t="s">
         <v>364</v>
       </c>
     </row>
     <row r="74" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C74" s="34"/>
-      <c r="D74" s="34"/>
+      <c r="C74" s="27"/>
+      <c r="D74" s="27"/>
     </row>
     <row r="75" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B75" s="34" t="s">
+      <c r="B75" s="27" t="s">
         <v>365</v>
       </c>
-      <c r="D75" s="34"/>
-      <c r="E75" s="45">
+      <c r="D75" s="27"/>
+      <c r="E75" s="38">
         <v>7420</v>
       </c>
-      <c r="F75" s="45">
+      <c r="F75" s="38">
         <v>7420</v>
       </c>
       <c r="G75" t="s">
@@ -5045,148 +5012,148 @@
       </c>
     </row>
     <row r="76" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C76" s="34"/>
-      <c r="D76" s="34"/>
+      <c r="C76" s="27"/>
+      <c r="D76" s="27"/>
     </row>
     <row r="77" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B77" s="34" t="s">
+      <c r="B77" s="27" t="s">
         <v>367</v>
       </c>
-      <c r="D77" s="34"/>
-      <c r="E77" s="36"/>
-      <c r="F77" s="36"/>
+      <c r="D77" s="27"/>
+      <c r="E77" s="29"/>
+      <c r="F77" s="29"/>
       <c r="G77" t="s">
         <v>368</v>
       </c>
     </row>
     <row r="78" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B78" s="34"/>
-      <c r="D78" s="34"/>
+      <c r="B78" s="27"/>
+      <c r="D78" s="27"/>
     </row>
     <row r="79" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B79" s="34" t="s">
+      <c r="B79" s="27" t="s">
         <v>369</v>
       </c>
-      <c r="D79" s="34"/>
-      <c r="E79" s="36"/>
-      <c r="F79" s="36"/>
+      <c r="D79" s="27"/>
+      <c r="E79" s="29"/>
+      <c r="F79" s="29"/>
       <c r="G79" t="s">
         <v>370</v>
       </c>
     </row>
     <row r="80" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B80" s="34"/>
-      <c r="D80" s="34"/>
+      <c r="B80" s="27"/>
+      <c r="D80" s="27"/>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B81" s="34" t="s">
+      <c r="B81" s="27" t="s">
         <v>371</v>
       </c>
-      <c r="D81" s="34"/>
-      <c r="E81" s="36"/>
-      <c r="F81" s="36"/>
+      <c r="D81" s="27"/>
+      <c r="E81" s="29"/>
+      <c r="F81" s="29"/>
       <c r="G81" t="s">
         <v>372</v>
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B82" s="34"/>
-      <c r="D82" s="34"/>
+      <c r="B82" s="27"/>
+      <c r="D82" s="27"/>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B83" s="34" t="s">
+      <c r="B83" s="27" t="s">
         <v>373</v>
       </c>
-      <c r="D83" s="34"/>
-      <c r="E83" s="36"/>
-      <c r="F83" s="36"/>
+      <c r="D83" s="27"/>
+      <c r="E83" s="29"/>
+      <c r="F83" s="29"/>
       <c r="G83" t="s">
         <v>374</v>
       </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C84" s="48"/>
-      <c r="D84" s="38"/>
-      <c r="E84" s="36"/>
-      <c r="F84" s="36"/>
+      <c r="C84" s="41"/>
+      <c r="D84" s="31"/>
+      <c r="E84" s="29"/>
+      <c r="F84" s="29"/>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C85" s="48"/>
-      <c r="D85" s="38"/>
-      <c r="E85" s="36"/>
-      <c r="F85" s="36"/>
+      <c r="C85" s="41"/>
+      <c r="D85" s="31"/>
+      <c r="E85" s="29"/>
+      <c r="F85" s="29"/>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C86" s="48"/>
-      <c r="D86" s="38"/>
-      <c r="E86" s="36"/>
-      <c r="F86" s="36"/>
+      <c r="C86" s="41"/>
+      <c r="D86" s="31"/>
+      <c r="E86" s="29"/>
+      <c r="F86" s="29"/>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C87" s="48"/>
-      <c r="D87" s="38"/>
-      <c r="E87" s="36"/>
-      <c r="F87" s="36"/>
+      <c r="C87" s="41"/>
+      <c r="D87" s="31"/>
+      <c r="E87" s="29"/>
+      <c r="F87" s="29"/>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C88" s="48"/>
-      <c r="D88" s="38"/>
-      <c r="E88" s="36"/>
-      <c r="F88" s="36"/>
+      <c r="C88" s="41"/>
+      <c r="D88" s="31"/>
+      <c r="E88" s="29"/>
+      <c r="F88" s="29"/>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C89" s="48"/>
-      <c r="D89" s="38"/>
-      <c r="E89" s="36"/>
-      <c r="F89" s="36"/>
+      <c r="C89" s="41"/>
+      <c r="D89" s="31"/>
+      <c r="E89" s="29"/>
+      <c r="F89" s="29"/>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C90" s="48"/>
-      <c r="D90" s="38"/>
-      <c r="E90" s="36"/>
-      <c r="F90" s="36"/>
+      <c r="C90" s="41"/>
+      <c r="D90" s="31"/>
+      <c r="E90" s="29"/>
+      <c r="F90" s="29"/>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C91" s="38"/>
-      <c r="D91" s="38"/>
-      <c r="E91" s="37"/>
-      <c r="F91" s="37"/>
+      <c r="C91" s="31"/>
+      <c r="D91" s="31"/>
+      <c r="E91" s="30"/>
+      <c r="F91" s="30"/>
     </row>
     <row r="92" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A92" s="52" t="s">
+      <c r="A92" s="45" t="s">
         <v>375</v>
       </c>
-      <c r="D92" s="52"/>
-      <c r="E92" s="53"/>
-      <c r="F92" s="53"/>
+      <c r="D92" s="45"/>
+      <c r="E92" s="46"/>
+      <c r="F92" s="46"/>
       <c r="G92" t="s">
         <v>376</v>
       </c>
     </row>
     <row r="93" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="C93" s="34"/>
-      <c r="D93" s="34"/>
+      <c r="C93" s="27"/>
+      <c r="D93" s="27"/>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A94" s="34" t="s">
+      <c r="A94" s="27" t="s">
         <v>377</v>
       </c>
-      <c r="D94" s="34"/>
-      <c r="E94" s="36"/>
-      <c r="F94" s="36"/>
+      <c r="D94" s="27"/>
+      <c r="E94" s="29"/>
+      <c r="F94" s="29"/>
       <c r="G94" t="s">
         <v>378</v>
       </c>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A95" s="34" t="s">
+      <c r="A95" s="27" t="s">
         <v>379</v>
       </c>
-      <c r="D95" s="34"/>
-      <c r="E95" s="44">
+      <c r="D95" s="27"/>
+      <c r="E95" s="37">
         <v>7500</v>
       </c>
-      <c r="F95" s="44">
+      <c r="F95" s="37">
         <v>7500</v>
       </c>
       <c r="G95" t="s">
@@ -5194,34 +5161,34 @@
       </c>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A96" s="34" t="s">
+      <c r="A96" s="27" t="s">
         <v>381</v>
       </c>
-      <c r="D96" s="34"/>
-      <c r="E96" s="42"/>
-      <c r="F96" s="42"/>
+      <c r="D96" s="27"/>
+      <c r="E96" s="35"/>
+      <c r="F96" s="35"/>
       <c r="G96" t="s">
         <v>382</v>
       </c>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A97" s="34" t="s">
+      <c r="A97" s="27" t="s">
         <v>383</v>
       </c>
-      <c r="D97" s="34"/>
-      <c r="E97" s="42"/>
-      <c r="F97" s="42"/>
+      <c r="D97" s="27"/>
+      <c r="E97" s="35"/>
+      <c r="F97" s="35"/>
       <c r="G97" t="s">
         <v>384</v>
       </c>
     </row>
     <row r="98" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A98" s="34" t="s">
+      <c r="A98" s="27" t="s">
         <v>385</v>
       </c>
-      <c r="D98" s="34"/>
-      <c r="E98" s="53"/>
-      <c r="F98" s="53"/>
+      <c r="D98" s="27"/>
+      <c r="E98" s="46"/>
+      <c r="F98" s="46"/>
       <c r="G98" t="s">
         <v>386</v>
       </c>
@@ -5232,6 +5199,39 @@
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
   <customProperties>
     <customPr name="OrphanNamesChecked" r:id="rId2"/>
+  </customProperties>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="Q17" sqref="Q17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>99</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <customProperties>
+    <customPr name="OrphanNamesChecked" r:id="rId1"/>
   </customProperties>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Updated f1 output formatter to include total and subtotal formulas in output. Updated mapping template in parameters.
</commit_message>
<xml_diff>
--- a/parameters/mas_forms_tb_mapping.xlsx
+++ b/parameters/mas_forms_tb_mapping.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6320" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6320"/>
   </bookViews>
   <sheets>
     <sheet name="Form 1 - TB mapping" sheetId="17" r:id="rId1"/>
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="865" uniqueCount="597">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="897" uniqueCount="629">
   <si>
     <t>Form 1 - Statement of assets and liabilities</t>
   </si>
@@ -1922,6 +1922,102 @@
   </si>
   <si>
     <t>unclassified31</t>
+  </si>
+  <si>
+    <t>= SUM(G10:G18)</t>
+  </si>
+  <si>
+    <t>= SUM(F12:F13)</t>
+  </si>
+  <si>
+    <t>= SUM(F27:F28)</t>
+  </si>
+  <si>
+    <t>= SUM(F32:F33)</t>
+  </si>
+  <si>
+    <t>= SUM(F35:F36)</t>
+  </si>
+  <si>
+    <t>= SUM(F39:F41)</t>
+  </si>
+  <si>
+    <t>= SUM(F47:F48)</t>
+  </si>
+  <si>
+    <t>= SUM(F54:F56)</t>
+  </si>
+  <si>
+    <t>= SUM(F64:F65)</t>
+  </si>
+  <si>
+    <t>=SUM(G25:G66)</t>
+  </si>
+  <si>
+    <t>= SUM(F71:F72)</t>
+  </si>
+  <si>
+    <t>= SUM(F75:F76)</t>
+  </si>
+  <si>
+    <t>= SUM(G68:G86)</t>
+  </si>
+  <si>
+    <t>= SUM(F92:F93)</t>
+  </si>
+  <si>
+    <t>= SUM(F96:F97)</t>
+  </si>
+  <si>
+    <t>= SUM(G92:G109)</t>
+  </si>
+  <si>
+    <t>= SUM(G88, G111)</t>
+  </si>
+  <si>
+    <t>= SUM(G20,G113)</t>
+  </si>
+  <si>
+    <t>= SUM(F122:F123)</t>
+  </si>
+  <si>
+    <t>= SUM(F129:F130)</t>
+  </si>
+  <si>
+    <t>= SUM(F134:F135)</t>
+  </si>
+  <si>
+    <t>= SUM(F146:F147)</t>
+  </si>
+  <si>
+    <t>= SUM(G120:G153)</t>
+  </si>
+  <si>
+    <t>= G155 - SUM(G156:G157)</t>
+  </si>
+  <si>
+    <t>= SUM(F161:F163)</t>
+  </si>
+  <si>
+    <t>= SUM(F168:F170)</t>
+  </si>
+  <si>
+    <t>= SUM(F173:F174)</t>
+  </si>
+  <si>
+    <t>= SUM(F181:F183)</t>
+  </si>
+  <si>
+    <t>= SUM(G158:G183)</t>
+  </si>
+  <si>
+    <t>= SUM(F191:F192)</t>
+  </si>
+  <si>
+    <t>= SUM(G188:G198)</t>
+  </si>
+  <si>
+    <t>= SUM(G185,G200)</t>
   </si>
 </sst>
 </file>
@@ -2356,7 +2452,7 @@
     <xf numFmtId="0" fontId="8" fillId="4" borderId="13"/>
     <xf numFmtId="43" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="102">
+  <cellXfs count="104">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2596,6 +2692,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -2908,8 +3010,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H238"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="E42" sqref="E42"/>
+    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="K68" sqref="K68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2932,10 +3034,10 @@
       <c r="E1" s="2"/>
     </row>
     <row r="2" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="95" t="s">
+      <c r="A2" s="97" t="s">
         <v>101</v>
       </c>
-      <c r="B2" s="96"/>
+      <c r="B2" s="98"/>
       <c r="C2" s="11" t="s">
         <v>251</v>
       </c>
@@ -2943,10 +3045,10 @@
       <c r="E2" s="3"/>
     </row>
     <row r="3" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A3" s="97" t="s">
+      <c r="A3" s="99" t="s">
         <v>102</v>
       </c>
-      <c r="B3" s="98"/>
+      <c r="B3" s="100"/>
       <c r="C3" s="12" t="s">
         <v>112</v>
       </c>
@@ -2954,10 +3056,10 @@
       <c r="E3" s="4"/>
     </row>
     <row r="4" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A4" s="97" t="s">
+      <c r="A4" s="99" t="s">
         <v>103</v>
       </c>
-      <c r="B4" s="98"/>
+      <c r="B4" s="100"/>
       <c r="C4" s="12" t="s">
         <v>111</v>
       </c>
@@ -2965,10 +3067,10 @@
       <c r="E4" s="4"/>
     </row>
     <row r="5" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="99" t="s">
+      <c r="A5" s="101" t="s">
         <v>104</v>
       </c>
-      <c r="B5" s="100"/>
+      <c r="B5" s="102"/>
       <c r="C5" s="13"/>
       <c r="D5" s="5"/>
       <c r="E5" s="5"/>
@@ -3036,7 +3138,9 @@
       <c r="F13" s="16">
         <v>6900.1</v>
       </c>
-      <c r="G13" s="3"/>
+      <c r="G13" s="95" t="s">
+        <v>598</v>
+      </c>
       <c r="H13" s="6" t="s">
         <v>155</v>
       </c>
@@ -3108,8 +3212,8 @@
       <c r="A20" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="G20" s="16">
-        <v>999999999</v>
+      <c r="G20" s="95" t="s">
+        <v>597</v>
       </c>
       <c r="H20" s="6" t="s">
         <v>252</v>
@@ -3119,10 +3223,10 @@
       <c r="G21" s="19"/>
     </row>
     <row r="22" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A22" s="101" t="s">
+      <c r="A22" s="103" t="s">
         <v>7</v>
       </c>
-      <c r="B22" s="101"/>
+      <c r="B22" s="103"/>
       <c r="C22" s="8"/>
       <c r="D22" s="8"/>
       <c r="E22" s="8"/>
@@ -3183,7 +3287,9 @@
       <c r="F28" s="16">
         <v>999999999</v>
       </c>
-      <c r="G28" s="16"/>
+      <c r="G28" s="95" t="s">
+        <v>599</v>
+      </c>
       <c r="H28" s="6" t="s">
         <v>163</v>
       </c>
@@ -3245,7 +3351,9 @@
       <c r="F33" s="16">
         <v>999999999</v>
       </c>
-      <c r="G33" s="16"/>
+      <c r="G33" s="95" t="s">
+        <v>600</v>
+      </c>
       <c r="H33" s="6" t="s">
         <v>167</v>
       </c>
@@ -3280,7 +3388,9 @@
       <c r="F36" s="16">
         <v>999999999</v>
       </c>
-      <c r="G36" s="16"/>
+      <c r="G36" s="95" t="s">
+        <v>601</v>
+      </c>
       <c r="H36" s="6" t="s">
         <v>169</v>
       </c>
@@ -3333,7 +3443,9 @@
       <c r="F41" s="16">
         <v>999999999</v>
       </c>
-      <c r="G41" s="16"/>
+      <c r="G41" s="95" t="s">
+        <v>602</v>
+      </c>
       <c r="H41" s="6" t="s">
         <v>172</v>
       </c>
@@ -3407,7 +3519,9 @@
       <c r="F48" s="16">
         <v>999999999</v>
       </c>
-      <c r="G48" s="16"/>
+      <c r="G48" s="95" t="s">
+        <v>603</v>
+      </c>
       <c r="H48" s="6" t="s">
         <v>176</v>
       </c>
@@ -3493,7 +3607,9 @@
       <c r="F56" s="16">
         <v>999999999</v>
       </c>
-      <c r="G56" s="16"/>
+      <c r="G56" s="95" t="s">
+        <v>604</v>
+      </c>
       <c r="H56" s="6" t="s">
         <v>181</v>
       </c>
@@ -3588,7 +3704,9 @@
       <c r="F65" s="16">
         <v>999999999</v>
       </c>
-      <c r="G65" s="16"/>
+      <c r="G65" s="95" t="s">
+        <v>605</v>
+      </c>
       <c r="H65" s="6" t="s">
         <v>186</v>
       </c>
@@ -3619,8 +3737,8 @@
       <c r="D68" s="7"/>
       <c r="E68" s="7"/>
       <c r="F68" s="19"/>
-      <c r="G68" s="16">
-        <v>999999999</v>
+      <c r="G68" s="95" t="s">
+        <v>606</v>
       </c>
       <c r="H68" s="6" t="s">
         <v>253</v>
@@ -3660,7 +3778,9 @@
       <c r="F72" s="16">
         <v>999999999</v>
       </c>
-      <c r="G72" s="3"/>
+      <c r="G72" s="95" t="s">
+        <v>607</v>
+      </c>
       <c r="H72" s="6" t="s">
         <v>189</v>
       </c>
@@ -3699,7 +3819,9 @@
       <c r="F76" s="16">
         <v>999999999</v>
       </c>
-      <c r="G76" s="3"/>
+      <c r="G76" s="95" t="s">
+        <v>608</v>
+      </c>
       <c r="H76" s="6" t="s">
         <v>191</v>
       </c>
@@ -3806,8 +3928,8 @@
       </c>
       <c r="D88" s="21"/>
       <c r="E88" s="21"/>
-      <c r="G88" s="16">
-        <v>999999999</v>
+      <c r="G88" s="95" t="s">
+        <v>609</v>
       </c>
       <c r="H88" s="6" t="s">
         <v>254</v>
@@ -3846,7 +3968,9 @@
       <c r="F93" s="16">
         <v>999999999</v>
       </c>
-      <c r="G93" s="3"/>
+      <c r="G93" s="95" t="s">
+        <v>610</v>
+      </c>
       <c r="H93" s="6" t="s">
         <v>247</v>
       </c>
@@ -3885,7 +4009,9 @@
       <c r="F97" s="16">
         <v>999999999</v>
       </c>
-      <c r="G97" s="3"/>
+      <c r="G97" s="95" t="s">
+        <v>611</v>
+      </c>
       <c r="H97" s="6" t="s">
         <v>198</v>
       </c>
@@ -4011,8 +4137,8 @@
       </c>
       <c r="D111" s="21"/>
       <c r="E111" s="21"/>
-      <c r="G111" s="16">
-        <v>999999999</v>
+      <c r="G111" s="95" t="s">
+        <v>612</v>
       </c>
       <c r="H111" s="6" t="s">
         <v>255</v>
@@ -4029,8 +4155,8 @@
       </c>
       <c r="D113" s="22"/>
       <c r="E113" s="22"/>
-      <c r="G113" s="16">
-        <v>999999999</v>
+      <c r="G113" s="95" t="s">
+        <v>613</v>
       </c>
       <c r="H113" s="6" t="s">
         <v>256</v>
@@ -4042,8 +4168,8 @@
       </c>
       <c r="D115" s="20"/>
       <c r="E115" s="20"/>
-      <c r="G115" s="16">
-        <v>999999999</v>
+      <c r="G115" s="95" t="s">
+        <v>614</v>
       </c>
       <c r="H115" s="6" t="s">
         <v>257</v>
@@ -4105,7 +4231,9 @@
       <c r="F123" s="16">
         <v>999999999</v>
       </c>
-      <c r="G123" s="3"/>
+      <c r="G123" s="95" t="s">
+        <v>615</v>
+      </c>
       <c r="H123" s="6" t="s">
         <v>207</v>
       </c>
@@ -4183,7 +4311,9 @@
       <c r="F130" s="16">
         <v>999999999</v>
       </c>
-      <c r="G130" s="3"/>
+      <c r="G130" s="95" t="s">
+        <v>616</v>
+      </c>
       <c r="H130" s="6" t="s">
         <v>213</v>
       </c>
@@ -4224,7 +4354,9 @@
       <c r="F135" s="16">
         <v>999999999</v>
       </c>
-      <c r="G135" s="3"/>
+      <c r="G135" s="95" t="s">
+        <v>617</v>
+      </c>
       <c r="H135" s="6" t="s">
         <v>215</v>
       </c>
@@ -4338,7 +4470,9 @@
       <c r="F147" s="16">
         <v>999999999</v>
       </c>
-      <c r="G147" s="3"/>
+      <c r="G147" s="95" t="s">
+        <v>618</v>
+      </c>
       <c r="H147" s="6" t="s">
         <v>222</v>
       </c>
@@ -4414,8 +4548,8 @@
       </c>
       <c r="D155" s="7"/>
       <c r="E155" s="7"/>
-      <c r="G155" s="16">
-        <v>999999999</v>
+      <c r="G155" s="95" t="s">
+        <v>619</v>
       </c>
       <c r="H155" s="6" t="s">
         <v>258</v>
@@ -4454,8 +4588,8 @@
       </c>
       <c r="D158" s="7"/>
       <c r="E158" s="7"/>
-      <c r="G158" s="16">
-        <v>999999999</v>
+      <c r="G158" s="95" t="s">
+        <v>620</v>
       </c>
       <c r="H158" s="6" t="s">
         <v>259</v>
@@ -4505,7 +4639,9 @@
       <c r="F163" s="16">
         <v>999999999</v>
       </c>
-      <c r="G163" s="3"/>
+      <c r="G163" s="95" t="s">
+        <v>621</v>
+      </c>
       <c r="H163" s="6" t="s">
         <v>230</v>
       </c>
@@ -4572,7 +4708,9 @@
       <c r="F170" s="16">
         <v>999999999</v>
       </c>
-      <c r="G170" s="3"/>
+      <c r="G170" s="95" t="s">
+        <v>622</v>
+      </c>
       <c r="H170" s="6" t="s">
         <v>235</v>
       </c>
@@ -4609,7 +4747,9 @@
       <c r="F174" s="16">
         <v>999999999</v>
       </c>
-      <c r="G174" s="3"/>
+      <c r="G174" s="95" t="s">
+        <v>623</v>
+      </c>
       <c r="H174" s="6" t="s">
         <v>237</v>
       </c>
@@ -4694,7 +4834,9 @@
       <c r="F183" s="16">
         <v>5200.2</v>
       </c>
-      <c r="G183" s="3"/>
+      <c r="G183" s="96" t="s">
+        <v>624</v>
+      </c>
       <c r="H183" s="6" t="s">
         <v>242</v>
       </c>
@@ -4710,8 +4852,8 @@
       </c>
       <c r="D185" s="21"/>
       <c r="E185" s="21"/>
-      <c r="G185" s="16">
-        <v>999999999</v>
+      <c r="G185" s="95" t="s">
+        <v>625</v>
       </c>
       <c r="H185" s="6" t="s">
         <v>260</v>
@@ -4770,7 +4912,9 @@
       <c r="F192" s="16">
         <v>999999999</v>
       </c>
-      <c r="G192" s="3"/>
+      <c r="G192" s="95" t="s">
+        <v>626</v>
+      </c>
       <c r="H192" s="6" t="s">
         <v>245</v>
       </c>
@@ -4840,8 +4984,8 @@
       </c>
       <c r="D200" s="21"/>
       <c r="E200" s="21"/>
-      <c r="G200" s="16">
-        <v>999999999</v>
+      <c r="G200" s="95" t="s">
+        <v>627</v>
       </c>
       <c r="H200" s="6" t="s">
         <v>261</v>
@@ -4860,8 +5004,8 @@
       <c r="C202" s="22"/>
       <c r="D202" s="22"/>
       <c r="E202" s="22"/>
-      <c r="G202" s="16">
-        <v>999999999</v>
+      <c r="G202" s="95" t="s">
+        <v>628</v>
       </c>
       <c r="H202" s="6" t="s">
         <v>262</v>
@@ -5253,8 +5397,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H132"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Updated f3 output formatter and template_reader and added formulas to form 3 template in parameters
</commit_message>
<xml_diff>
--- a/parameters/mas_forms_tb_mapping.xlsx
+++ b/parameters/mas_forms_tb_mapping.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6320"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6320" firstSheet="2" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Form 1 - TB mapping" sheetId="17" r:id="rId1"/>
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="897" uniqueCount="629">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="897" uniqueCount="660">
   <si>
     <t>Form 1 - Statement of assets and liabilities</t>
   </si>
@@ -2018,6 +2018,99 @@
   </si>
   <si>
     <t>= SUM(G185,G200)</t>
+  </si>
+  <si>
+    <t>&lt;&lt;&lt;Taken from Form 1&gt;&gt;&gt;</t>
+  </si>
+  <si>
+    <t>= SUM(E10:E11)</t>
+  </si>
+  <si>
+    <t>= SUM(F11:F13) - SUM(F14:F15)</t>
+  </si>
+  <si>
+    <t>= SUM(F16:F17)</t>
+  </si>
+  <si>
+    <t>= SUM(F32:F41)</t>
+  </si>
+  <si>
+    <t>= SUM(F21:F29) - F42</t>
+  </si>
+  <si>
+    <t>= SUM(E47:E48)</t>
+  </si>
+  <si>
+    <t>= SUM(E54:E56)</t>
+  </si>
+  <si>
+    <t>= SUM(F56:F66)</t>
+  </si>
+  <si>
+    <t>= SUM(F71:F78)</t>
+  </si>
+  <si>
+    <t>= SUM(F82:F84)</t>
+  </si>
+  <si>
+    <t>= SUM(F89:F90)</t>
+  </si>
+  <si>
+    <t>= SUM(F50,F68,F79,F86,F92)</t>
+  </si>
+  <si>
+    <t>= F48</t>
+  </si>
+  <si>
+    <t>= F43/F96 * 100%</t>
+  </si>
+  <si>
+    <t>= F100 - SUM(F102:F109)</t>
+  </si>
+  <si>
+    <t>= SUM(F111:F113) - F115</t>
+  </si>
+  <si>
+    <t>= F110 / F116 * 100%</t>
+  </si>
+  <si>
+    <t>= F42</t>
+  </si>
+  <si>
+    <t>= SUM(E126:E127)</t>
+  </si>
+  <si>
+    <t>= SUM(F121:F122) - SUM(F124:F129)</t>
+  </si>
+  <si>
+    <t>= MIN(F43 * 100, 10000000)</t>
+  </si>
+  <si>
+    <t>= SUM(E8:E49)</t>
+  </si>
+  <si>
+    <t>= SUM(F8:F49)</t>
+  </si>
+  <si>
+    <t>= SUM(F60:F83)</t>
+  </si>
+  <si>
+    <t>= SUM(E60:E83)</t>
+  </si>
+  <si>
+    <t>= E57 - E92</t>
+  </si>
+  <si>
+    <t>= F57 - F92</t>
+  </si>
+  <si>
+    <t>= F94 - F95</t>
+  </si>
+  <si>
+    <t>= E94 - E95</t>
+  </si>
+  <si>
+    <t>= SUM(E96:E97)</t>
   </si>
 </sst>
 </file>
@@ -2452,7 +2545,7 @@
     <xf numFmtId="0" fontId="8" fillId="4" borderId="13"/>
     <xf numFmtId="43" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="104">
+  <cellXfs count="105">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2719,6 +2812,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Comma" xfId="3" builtinId="3"/>
@@ -3010,8 +3104,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H238"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="K68" sqref="K68"/>
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5397,13 +5491,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H132"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+    <sheetView topLeftCell="D108" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G140" sqref="G140"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="4" max="4" width="79.7265625" customWidth="1"/>
+    <col min="5" max="6" width="22.90625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9.1796875" style="90"/>
   </cols>
   <sheetData>
@@ -5529,7 +5624,7 @@
         <v>391</v>
       </c>
       <c r="E10" s="88" t="s">
-        <v>538</v>
+        <v>629</v>
       </c>
       <c r="F10" s="55"/>
       <c r="G10" s="91" t="s">
@@ -5545,10 +5640,10 @@
         <v>392</v>
       </c>
       <c r="E11" s="88" t="s">
-        <v>538</v>
+        <v>629</v>
       </c>
       <c r="F11" s="88" t="s">
-        <v>538</v>
+        <v>630</v>
       </c>
       <c r="G11" s="76" t="s">
         <v>155</v>
@@ -5564,7 +5659,7 @@
       <c r="D12" s="55"/>
       <c r="E12" s="55"/>
       <c r="F12" s="88" t="s">
-        <v>538</v>
+        <v>629</v>
       </c>
       <c r="G12" s="76" t="s">
         <v>157</v>
@@ -5580,7 +5675,7 @@
       <c r="D13" s="55"/>
       <c r="E13" s="55"/>
       <c r="F13" s="88" t="s">
-        <v>538</v>
+        <v>629</v>
       </c>
       <c r="G13" s="76" t="s">
         <v>158</v>
@@ -5630,7 +5725,7 @@
       <c r="D16" s="55"/>
       <c r="E16" s="55"/>
       <c r="F16" s="88" t="s">
-        <v>538</v>
+        <v>631</v>
       </c>
       <c r="G16" s="76" t="s">
         <v>400</v>
@@ -5646,7 +5741,7 @@
       <c r="D17" s="55"/>
       <c r="E17" s="55"/>
       <c r="F17" s="88" t="s">
-        <v>538</v>
+        <v>629</v>
       </c>
       <c r="G17" s="76" t="s">
         <v>160</v>
@@ -5662,7 +5757,7 @@
       <c r="D18" s="55"/>
       <c r="E18" s="55"/>
       <c r="F18" s="88" t="s">
-        <v>538</v>
+        <v>632</v>
       </c>
       <c r="G18" s="90" t="s">
         <v>403</v>
@@ -5699,7 +5794,7 @@
       <c r="D21" s="55"/>
       <c r="E21" s="55"/>
       <c r="F21" s="88" t="s">
-        <v>538</v>
+        <v>632</v>
       </c>
       <c r="G21" s="90" t="s">
         <v>406</v>
@@ -5726,7 +5821,7 @@
       </c>
       <c r="E23" s="55"/>
       <c r="F23" s="88" t="s">
-        <v>538</v>
+        <v>629</v>
       </c>
       <c r="G23" s="76" t="s">
         <v>154</v>
@@ -5742,7 +5837,7 @@
       </c>
       <c r="E24" s="55"/>
       <c r="F24" s="88" t="s">
-        <v>538</v>
+        <v>629</v>
       </c>
       <c r="G24" s="90" t="s">
         <v>410</v>
@@ -5774,7 +5869,7 @@
       </c>
       <c r="E26" s="55"/>
       <c r="F26" s="88" t="s">
-        <v>538</v>
+        <v>629</v>
       </c>
       <c r="G26" s="76" t="s">
         <v>156</v>
@@ -5790,7 +5885,7 @@
       </c>
       <c r="E27" s="55"/>
       <c r="F27" s="88" t="s">
-        <v>538</v>
+        <v>629</v>
       </c>
       <c r="G27" s="76" t="s">
         <v>159</v>
@@ -5860,7 +5955,7 @@
       </c>
       <c r="E32" s="55"/>
       <c r="F32" s="88" t="s">
-        <v>538</v>
+        <v>629</v>
       </c>
       <c r="G32" s="76" t="s">
         <v>249</v>
@@ -5892,7 +5987,7 @@
       </c>
       <c r="E34" s="55"/>
       <c r="F34" s="88" t="s">
-        <v>538</v>
+        <v>629</v>
       </c>
       <c r="G34" s="76" t="s">
         <v>241</v>
@@ -5924,7 +6019,7 @@
       </c>
       <c r="E36" s="55"/>
       <c r="F36" s="88" t="s">
-        <v>538</v>
+        <v>629</v>
       </c>
       <c r="G36" s="90" t="s">
         <v>427</v>
@@ -5972,7 +6067,7 @@
       </c>
       <c r="E39" s="55"/>
       <c r="F39" s="88" t="s">
-        <v>538</v>
+        <v>629</v>
       </c>
       <c r="G39" s="90" t="s">
         <v>433</v>
@@ -6020,7 +6115,7 @@
       <c r="D42" s="55"/>
       <c r="E42" s="55"/>
       <c r="F42" s="88" t="s">
-        <v>538</v>
+        <v>633</v>
       </c>
       <c r="G42" s="91" t="s">
         <v>438</v>
@@ -6036,7 +6131,7 @@
       <c r="D43" s="55"/>
       <c r="E43" s="55"/>
       <c r="F43" s="88" t="s">
-        <v>538</v>
+        <v>634</v>
       </c>
       <c r="G43" s="91" t="s">
         <v>440</v>
@@ -6103,7 +6198,7 @@
         <v>538</v>
       </c>
       <c r="F48" s="88" t="s">
-        <v>538</v>
+        <v>635</v>
       </c>
       <c r="G48" s="90" t="s">
         <v>446</v>
@@ -6125,7 +6220,7 @@
       <c r="D50" s="43"/>
       <c r="E50" s="43"/>
       <c r="F50" s="88" t="s">
-        <v>538</v>
+        <v>642</v>
       </c>
       <c r="G50" s="90" t="s">
         <v>448</v>
@@ -6196,7 +6291,7 @@
         <v>538</v>
       </c>
       <c r="F56" s="88" t="s">
-        <v>538</v>
+        <v>636</v>
       </c>
       <c r="G56" s="90" t="s">
         <v>553</v>
@@ -6368,7 +6463,7 @@
       <c r="D68" s="43"/>
       <c r="E68" s="43"/>
       <c r="F68" s="88" t="s">
-        <v>538</v>
+        <v>637</v>
       </c>
       <c r="G68" s="90" t="s">
         <v>564</v>
@@ -6521,7 +6616,7 @@
       <c r="D79" s="43"/>
       <c r="E79" s="43"/>
       <c r="F79" s="88" t="s">
-        <v>538</v>
+        <v>638</v>
       </c>
       <c r="G79" s="90" t="s">
         <v>573</v>
@@ -6603,7 +6698,7 @@
       <c r="D86" s="43"/>
       <c r="E86" s="43"/>
       <c r="F86" s="88" t="s">
-        <v>538</v>
+        <v>639</v>
       </c>
       <c r="G86" s="90" t="s">
         <v>577</v>
@@ -6670,7 +6765,7 @@
       <c r="D92" s="43"/>
       <c r="E92" s="43"/>
       <c r="F92" s="88" t="s">
-        <v>538</v>
+        <v>640</v>
       </c>
       <c r="G92" s="90" t="s">
         <v>580</v>
@@ -6718,7 +6813,7 @@
       <c r="D96" s="43"/>
       <c r="E96" s="43"/>
       <c r="F96" s="88" t="s">
-        <v>538</v>
+        <v>641</v>
       </c>
       <c r="G96" s="90" t="s">
         <v>487</v>
@@ -6733,7 +6828,7 @@
       <c r="D97" s="43"/>
       <c r="E97" s="43"/>
       <c r="F97" s="88" t="s">
-        <v>538</v>
+        <v>643</v>
       </c>
       <c r="G97" s="90" t="s">
         <v>489</v>
@@ -6893,7 +6988,7 @@
       <c r="D110" s="43"/>
       <c r="E110" s="43"/>
       <c r="F110" s="88" t="s">
-        <v>538</v>
+        <v>644</v>
       </c>
       <c r="G110" s="90" t="s">
         <v>590</v>
@@ -6967,7 +7062,7 @@
       <c r="D116" s="43"/>
       <c r="E116" s="43"/>
       <c r="F116" s="88" t="s">
-        <v>538</v>
+        <v>645</v>
       </c>
       <c r="G116" s="90" t="s">
         <v>594</v>
@@ -6982,7 +7077,7 @@
       <c r="D117" s="43"/>
       <c r="E117" s="43"/>
       <c r="F117" s="88" t="s">
-        <v>538</v>
+        <v>646</v>
       </c>
       <c r="G117" s="90" t="s">
         <v>595</v>
@@ -7017,7 +7112,7 @@
       <c r="D121" s="43"/>
       <c r="E121" s="43"/>
       <c r="F121" s="88" t="s">
-        <v>538</v>
+        <v>629</v>
       </c>
       <c r="G121" s="90" t="s">
         <v>262</v>
@@ -7057,7 +7152,7 @@
       <c r="D124" s="43"/>
       <c r="E124" s="43"/>
       <c r="F124" s="88" t="s">
-        <v>538</v>
+        <v>647</v>
       </c>
       <c r="G124" s="91" t="s">
         <v>512</v>
@@ -7099,7 +7194,7 @@
         <v>538</v>
       </c>
       <c r="F127" s="88" t="s">
-        <v>538</v>
+        <v>648</v>
       </c>
       <c r="G127" s="90" t="s">
         <v>517</v>
@@ -7144,7 +7239,7 @@
       <c r="D130" s="43"/>
       <c r="E130" s="43"/>
       <c r="F130" s="88" t="s">
-        <v>538</v>
+        <v>649</v>
       </c>
       <c r="G130" s="90" t="s">
         <v>523</v>
@@ -7174,7 +7269,7 @@
       <c r="D132" s="43"/>
       <c r="E132" s="43"/>
       <c r="F132" s="88" t="s">
-        <v>538</v>
+        <v>650</v>
       </c>
       <c r="G132" s="90" t="s">
         <v>527</v>
@@ -7306,8 +7401,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A4:G98"/>
   <sheetViews>
-    <sheetView zoomScale="82" workbookViewId="0">
-      <selection activeCell="H29" sqref="H29"/>
+    <sheetView tabSelected="1" topLeftCell="A61" zoomScale="82" workbookViewId="0">
+      <selection activeCell="K97" sqref="K97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -7911,10 +8006,10 @@
       </c>
       <c r="D57" s="41"/>
       <c r="E57" s="88" t="s">
-        <v>538</v>
+        <v>651</v>
       </c>
       <c r="F57" s="88" t="s">
-        <v>538</v>
+        <v>652</v>
       </c>
       <c r="G57" t="s">
         <v>345</v>
@@ -8264,10 +8359,10 @@
       </c>
       <c r="D92" s="42"/>
       <c r="E92" s="88" t="s">
-        <v>538</v>
+        <v>654</v>
       </c>
       <c r="F92" s="88" t="s">
-        <v>538</v>
+        <v>653</v>
       </c>
       <c r="G92" t="s">
         <v>376</v>
@@ -8283,10 +8378,10 @@
       </c>
       <c r="D94" s="27"/>
       <c r="E94" s="88" t="s">
-        <v>538</v>
+        <v>655</v>
       </c>
       <c r="F94" s="88" t="s">
-        <v>538</v>
+        <v>656</v>
       </c>
       <c r="G94" t="s">
         <v>378</v>
@@ -8312,11 +8407,11 @@
         <v>381</v>
       </c>
       <c r="D96" s="27"/>
-      <c r="E96" s="88" t="s">
-        <v>538</v>
-      </c>
-      <c r="F96" s="88" t="s">
-        <v>538</v>
+      <c r="E96" s="104" t="s">
+        <v>658</v>
+      </c>
+      <c r="F96" s="104" t="s">
+        <v>657</v>
       </c>
       <c r="G96" t="s">
         <v>382</v>
@@ -8342,11 +8437,11 @@
         <v>385</v>
       </c>
       <c r="D98" s="27"/>
-      <c r="E98" s="88" t="s">
-        <v>538</v>
-      </c>
-      <c r="F98" s="88" t="s">
-        <v>538</v>
+      <c r="E98" s="104" t="s">
+        <v>659</v>
+      </c>
+      <c r="F98" s="104" t="s">
+        <v>611</v>
       </c>
       <c r="G98" t="s">
         <v>386</v>

</xml_diff>

<commit_message>
Updated f2 output formatter and mapping template. Updated template_reader form1
</commit_message>
<xml_diff>
--- a/parameters/mas_forms_tb_mapping.xlsx
+++ b/parameters/mas_forms_tb_mapping.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6320" firstSheet="2" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6320" firstSheet="2" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Form 1 - TB mapping" sheetId="17" r:id="rId1"/>
@@ -17,6 +17,9 @@
     <sheet name="AR AP ageing template" sheetId="11" state="hidden" r:id="rId8"/>
     <sheet name="RPT template" sheetId="12" state="hidden" r:id="rId9"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Form 2 - TB mapping'!$F$1:$F$132</definedName>
+  </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -2062,18 +2065,12 @@
     <t>= F48</t>
   </si>
   <si>
-    <t>= F43/F96 * 100%</t>
-  </si>
-  <si>
     <t>= F100 - SUM(F102:F109)</t>
   </si>
   <si>
     <t>= SUM(F111:F113) - F115</t>
   </si>
   <si>
-    <t>= F110 / F116 * 100%</t>
-  </si>
-  <si>
     <t>= F42</t>
   </si>
   <si>
@@ -2111,6 +2108,12 @@
   </si>
   <si>
     <t>= SUM(E96:E97)</t>
+  </si>
+  <si>
+    <t>= F43/F96 * 100</t>
+  </si>
+  <si>
+    <t>= F110 / F116 * 100</t>
   </si>
 </sst>
 </file>
@@ -2791,6 +2794,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -2812,7 +2816,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Comma" xfId="3" builtinId="3"/>
@@ -3128,10 +3131,10 @@
       <c r="E1" s="2"/>
     </row>
     <row r="2" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="97" t="s">
+      <c r="A2" s="98" t="s">
         <v>101</v>
       </c>
-      <c r="B2" s="98"/>
+      <c r="B2" s="99"/>
       <c r="C2" s="11" t="s">
         <v>251</v>
       </c>
@@ -3139,10 +3142,10 @@
       <c r="E2" s="3"/>
     </row>
     <row r="3" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A3" s="99" t="s">
+      <c r="A3" s="100" t="s">
         <v>102</v>
       </c>
-      <c r="B3" s="100"/>
+      <c r="B3" s="101"/>
       <c r="C3" s="12" t="s">
         <v>112</v>
       </c>
@@ -3150,10 +3153,10 @@
       <c r="E3" s="4"/>
     </row>
     <row r="4" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A4" s="99" t="s">
+      <c r="A4" s="100" t="s">
         <v>103</v>
       </c>
-      <c r="B4" s="100"/>
+      <c r="B4" s="101"/>
       <c r="C4" s="12" t="s">
         <v>111</v>
       </c>
@@ -3161,10 +3164,10 @@
       <c r="E4" s="4"/>
     </row>
     <row r="5" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="101" t="s">
+      <c r="A5" s="102" t="s">
         <v>104</v>
       </c>
-      <c r="B5" s="102"/>
+      <c r="B5" s="103"/>
       <c r="C5" s="13"/>
       <c r="D5" s="5"/>
       <c r="E5" s="5"/>
@@ -3317,10 +3320,10 @@
       <c r="G21" s="19"/>
     </row>
     <row r="22" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A22" s="103" t="s">
+      <c r="A22" s="104" t="s">
         <v>7</v>
       </c>
-      <c r="B22" s="103"/>
+      <c r="B22" s="104"/>
       <c r="C22" s="8"/>
       <c r="D22" s="8"/>
       <c r="E22" s="8"/>
@@ -5491,8 +5494,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H132"/>
   <sheetViews>
-    <sheetView topLeftCell="D108" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G140" sqref="G140"/>
+    <sheetView tabSelected="1" topLeftCell="A88" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="N117" sqref="N117"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6828,7 +6831,7 @@
       <c r="D97" s="43"/>
       <c r="E97" s="43"/>
       <c r="F97" s="88" t="s">
-        <v>643</v>
+        <v>658</v>
       </c>
       <c r="G97" s="90" t="s">
         <v>489</v>
@@ -6988,7 +6991,7 @@
       <c r="D110" s="43"/>
       <c r="E110" s="43"/>
       <c r="F110" s="88" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="G110" s="90" t="s">
         <v>590</v>
@@ -7062,7 +7065,7 @@
       <c r="D116" s="43"/>
       <c r="E116" s="43"/>
       <c r="F116" s="88" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="G116" s="90" t="s">
         <v>594</v>
@@ -7077,7 +7080,7 @@
       <c r="D117" s="43"/>
       <c r="E117" s="43"/>
       <c r="F117" s="88" t="s">
-        <v>646</v>
+        <v>659</v>
       </c>
       <c r="G117" s="90" t="s">
         <v>595</v>
@@ -7152,7 +7155,7 @@
       <c r="D124" s="43"/>
       <c r="E124" s="43"/>
       <c r="F124" s="88" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="G124" s="91" t="s">
         <v>512</v>
@@ -7194,7 +7197,7 @@
         <v>538</v>
       </c>
       <c r="F127" s="88" t="s">
-        <v>648</v>
+        <v>646</v>
       </c>
       <c r="G127" s="90" t="s">
         <v>517</v>
@@ -7239,7 +7242,7 @@
       <c r="D130" s="43"/>
       <c r="E130" s="43"/>
       <c r="F130" s="88" t="s">
-        <v>649</v>
+        <v>647</v>
       </c>
       <c r="G130" s="90" t="s">
         <v>523</v>
@@ -7269,7 +7272,7 @@
       <c r="D132" s="43"/>
       <c r="E132" s="43"/>
       <c r="F132" s="88" t="s">
-        <v>650</v>
+        <v>648</v>
       </c>
       <c r="G132" s="90" t="s">
         <v>527</v>
@@ -7401,7 +7404,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A4:G98"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" zoomScale="82" workbookViewId="0">
+    <sheetView topLeftCell="A61" zoomScale="82" workbookViewId="0">
       <selection activeCell="K97" sqref="K97"/>
     </sheetView>
   </sheetViews>
@@ -8006,10 +8009,10 @@
       </c>
       <c r="D57" s="41"/>
       <c r="E57" s="88" t="s">
-        <v>651</v>
+        <v>649</v>
       </c>
       <c r="F57" s="88" t="s">
-        <v>652</v>
+        <v>650</v>
       </c>
       <c r="G57" t="s">
         <v>345</v>
@@ -8359,10 +8362,10 @@
       </c>
       <c r="D92" s="42"/>
       <c r="E92" s="88" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
       <c r="F92" s="88" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
       <c r="G92" t="s">
         <v>376</v>
@@ -8378,10 +8381,10 @@
       </c>
       <c r="D94" s="27"/>
       <c r="E94" s="88" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
       <c r="F94" s="88" t="s">
-        <v>656</v>
+        <v>654</v>
       </c>
       <c r="G94" t="s">
         <v>378</v>
@@ -8407,11 +8410,11 @@
         <v>381</v>
       </c>
       <c r="D96" s="27"/>
-      <c r="E96" s="104" t="s">
-        <v>658</v>
-      </c>
-      <c r="F96" s="104" t="s">
-        <v>657</v>
+      <c r="E96" s="97" t="s">
+        <v>656</v>
+      </c>
+      <c r="F96" s="97" t="s">
+        <v>655</v>
       </c>
       <c r="G96" t="s">
         <v>382</v>
@@ -8437,10 +8440,10 @@
         <v>385</v>
       </c>
       <c r="D98" s="27"/>
-      <c r="E98" s="104" t="s">
-        <v>659</v>
-      </c>
-      <c r="F98" s="104" t="s">
+      <c r="E98" s="97" t="s">
+        <v>657</v>
+      </c>
+      <c r="F98" s="97" t="s">
         <v>611</v>
       </c>
       <c r="G98" t="s">

</xml_diff>

<commit_message>
Renamed funds-related files, updated some form 1 logic as per DIC request
</commit_message>
<xml_diff>
--- a/parameters/mas_forms_tb_mapping.xlsx
+++ b/parameters/mas_forms_tb_mapping.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6320" firstSheet="2" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6320"/>
   </bookViews>
   <sheets>
     <sheet name="Form 1 - TB mapping" sheetId="17" r:id="rId1"/>
@@ -3107,8 +3107,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H238"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+    <sheetView tabSelected="1" topLeftCell="A178" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="K202" sqref="K202"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3712,8 +3712,8 @@
       </c>
     </row>
     <row r="57" spans="3:8" x14ac:dyDescent="0.35">
-      <c r="D57" s="7" t="s">
-        <v>31</v>
+      <c r="D57" s="49" t="s">
+        <v>28</v>
       </c>
       <c r="E57" s="7"/>
       <c r="F57" s="19"/>
@@ -5007,7 +5007,7 @@
       </c>
       <c r="E192" s="7"/>
       <c r="F192" s="16">
-        <v>999999999</v>
+        <v>5100.2</v>
       </c>
       <c r="G192" s="95" t="s">
         <v>626</v>
@@ -5494,7 +5494,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H132"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A88" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A88" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="N117" sqref="N117"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Added f2_checker, modified form3_part2 to add a catchall significant account field for other rev and other exp, modified form3_part1's other_revenue field calculation but pending confirmation of logic
</commit_message>
<xml_diff>
--- a/parameters/mas_forms_tb_mapping.xlsx
+++ b/parameters/mas_forms_tb_mapping.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6320" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12450" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Form 1 - TB mapping" sheetId="17" r:id="rId1"/>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="897" uniqueCount="660">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="897" uniqueCount="659">
   <si>
     <t>Form 1 - Statement of assets and liabilities</t>
   </si>
@@ -927,9 +927,6 @@
     <t>Current year
 &lt;&lt;&lt;current_fy&gt;&gt;&gt;
 $</t>
-  </si>
-  <si>
-    <t xml:space="preserve">var_name </t>
   </si>
   <si>
     <t>(1) Revenue -</t>
@@ -3236,7 +3233,7 @@
         <v>6900.1</v>
       </c>
       <c r="G13" s="95" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="H13" s="6" t="s">
         <v>155</v>
@@ -3310,7 +3307,7 @@
         <v>6</v>
       </c>
       <c r="G20" s="95" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="H20" s="6" t="s">
         <v>252</v>
@@ -3385,7 +3382,7 @@
         <v>999999999</v>
       </c>
       <c r="G28" s="95" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="H28" s="6" t="s">
         <v>163</v>
@@ -3449,7 +3446,7 @@
         <v>999999999</v>
       </c>
       <c r="G33" s="95" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="H33" s="6" t="s">
         <v>167</v>
@@ -3486,7 +3483,7 @@
         <v>999999999</v>
       </c>
       <c r="G36" s="95" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="H36" s="6" t="s">
         <v>169</v>
@@ -3541,7 +3538,7 @@
         <v>999999999</v>
       </c>
       <c r="G41" s="95" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="H41" s="6" t="s">
         <v>172</v>
@@ -3617,7 +3614,7 @@
         <v>999999999</v>
       </c>
       <c r="G48" s="95" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="H48" s="6" t="s">
         <v>176</v>
@@ -3705,7 +3702,7 @@
         <v>999999999</v>
       </c>
       <c r="G56" s="95" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="H56" s="6" t="s">
         <v>181</v>
@@ -3802,7 +3799,7 @@
         <v>999999999</v>
       </c>
       <c r="G65" s="95" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="H65" s="6" t="s">
         <v>186</v>
@@ -3835,7 +3832,7 @@
       <c r="E68" s="7"/>
       <c r="F68" s="19"/>
       <c r="G68" s="95" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="H68" s="6" t="s">
         <v>253</v>
@@ -3876,7 +3873,7 @@
         <v>999999999</v>
       </c>
       <c r="G72" s="95" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="H72" s="6" t="s">
         <v>189</v>
@@ -3917,7 +3914,7 @@
         <v>999999999</v>
       </c>
       <c r="G76" s="95" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="H76" s="6" t="s">
         <v>191</v>
@@ -4026,7 +4023,7 @@
       <c r="D88" s="21"/>
       <c r="E88" s="21"/>
       <c r="G88" s="95" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="H88" s="6" t="s">
         <v>254</v>
@@ -4066,7 +4063,7 @@
         <v>999999999</v>
       </c>
       <c r="G93" s="95" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="H93" s="6" t="s">
         <v>247</v>
@@ -4107,7 +4104,7 @@
         <v>999999999</v>
       </c>
       <c r="G97" s="95" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="H97" s="6" t="s">
         <v>198</v>
@@ -4235,7 +4232,7 @@
       <c r="D111" s="21"/>
       <c r="E111" s="21"/>
       <c r="G111" s="95" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="H111" s="6" t="s">
         <v>255</v>
@@ -4253,7 +4250,7 @@
       <c r="D113" s="22"/>
       <c r="E113" s="22"/>
       <c r="G113" s="95" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="H113" s="6" t="s">
         <v>256</v>
@@ -4266,7 +4263,7 @@
       <c r="D115" s="20"/>
       <c r="E115" s="20"/>
       <c r="G115" s="95" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="H115" s="6" t="s">
         <v>257</v>
@@ -4329,7 +4326,7 @@
         <v>999999999</v>
       </c>
       <c r="G123" s="95" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="H123" s="6" t="s">
         <v>207</v>
@@ -4409,7 +4406,7 @@
         <v>999999999</v>
       </c>
       <c r="G130" s="95" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="H130" s="6" t="s">
         <v>213</v>
@@ -4452,7 +4449,7 @@
         <v>999999999</v>
       </c>
       <c r="G135" s="95" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="H135" s="6" t="s">
         <v>215</v>
@@ -4568,7 +4565,7 @@
         <v>999999999</v>
       </c>
       <c r="G147" s="95" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="H147" s="6" t="s">
         <v>222</v>
@@ -4646,7 +4643,7 @@
       <c r="D155" s="7"/>
       <c r="E155" s="7"/>
       <c r="G155" s="95" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="H155" s="6" t="s">
         <v>258</v>
@@ -4686,7 +4683,7 @@
       <c r="D158" s="7"/>
       <c r="E158" s="7"/>
       <c r="G158" s="95" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="H158" s="6" t="s">
         <v>259</v>
@@ -4737,7 +4734,7 @@
         <v>999999999</v>
       </c>
       <c r="G163" s="95" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="H163" s="6" t="s">
         <v>230</v>
@@ -4806,7 +4803,7 @@
         <v>999999999</v>
       </c>
       <c r="G170" s="95" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="H170" s="6" t="s">
         <v>235</v>
@@ -4845,7 +4842,7 @@
         <v>999999999</v>
       </c>
       <c r="G174" s="95" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="H174" s="6" t="s">
         <v>237</v>
@@ -4932,7 +4929,7 @@
         <v>5200.2</v>
       </c>
       <c r="G183" s="96" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="H183" s="6" t="s">
         <v>242</v>
@@ -4950,7 +4947,7 @@
       <c r="D185" s="21"/>
       <c r="E185" s="21"/>
       <c r="G185" s="95" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="H185" s="6" t="s">
         <v>260</v>
@@ -5010,7 +5007,7 @@
         <v>5100.2</v>
       </c>
       <c r="G192" s="95" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="H192" s="6" t="s">
         <v>245</v>
@@ -5082,7 +5079,7 @@
       <c r="D200" s="21"/>
       <c r="E200" s="21"/>
       <c r="G200" s="95" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="H200" s="6" t="s">
         <v>261</v>
@@ -5102,7 +5099,7 @@
       <c r="D202" s="22"/>
       <c r="E202" s="22"/>
       <c r="G202" s="95" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="H202" s="6" t="s">
         <v>262</v>
@@ -5494,7 +5491,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H132"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A97" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="A120" sqref="A120"/>
     </sheetView>
   </sheetViews>
@@ -5507,7 +5504,7 @@
   <sheetData>
     <row r="1" spans="1:8" ht="26.5" thickBot="1" x14ac:dyDescent="0.65">
       <c r="A1" s="50" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="B1" s="51"/>
       <c r="C1" s="44"/>
@@ -5523,7 +5520,7 @@
       </c>
       <c r="B2" s="59"/>
       <c r="C2" s="52" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="D2" s="45"/>
       <c r="E2" s="45"/>
@@ -5599,7 +5596,7 @@
     </row>
     <row r="8" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A8" s="57" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="B8" s="57"/>
       <c r="C8" s="55"/>
@@ -5612,7 +5609,7 @@
       <c r="A9" s="55"/>
       <c r="B9" s="43"/>
       <c r="C9" s="64" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="D9" s="55"/>
       <c r="E9" s="55"/>
@@ -5624,10 +5621,10 @@
       <c r="B10" s="43"/>
       <c r="C10" s="55"/>
       <c r="D10" s="49" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="E10" s="88" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="F10" s="55"/>
       <c r="G10" s="91" t="s">
@@ -5640,13 +5637,13 @@
       <c r="B11" s="43"/>
       <c r="C11" s="55"/>
       <c r="D11" s="49" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="E11" s="88" t="s">
+        <v>627</v>
+      </c>
+      <c r="F11" s="88" t="s">
         <v>628</v>
-      </c>
-      <c r="F11" s="88" t="s">
-        <v>629</v>
       </c>
       <c r="G11" s="76" t="s">
         <v>155</v>
@@ -5657,12 +5654,12 @@
       <c r="A12" s="55"/>
       <c r="B12" s="43"/>
       <c r="C12" s="55" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="D12" s="55"/>
       <c r="E12" s="55"/>
       <c r="F12" s="88" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="G12" s="76" t="s">
         <v>157</v>
@@ -5673,12 +5670,12 @@
       <c r="A13" s="55"/>
       <c r="B13" s="43"/>
       <c r="C13" s="65" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="D13" s="55"/>
       <c r="E13" s="55"/>
       <c r="F13" s="88" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="G13" s="76" t="s">
         <v>158</v>
@@ -5692,14 +5689,14 @@
         <v>115</v>
       </c>
       <c r="D14" s="65" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="E14" s="55"/>
       <c r="F14" s="88" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="G14" s="90" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="H14" s="48"/>
     </row>
@@ -5708,14 +5705,14 @@
       <c r="B15" s="43"/>
       <c r="C15" s="55"/>
       <c r="D15" s="65" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="E15" s="55"/>
       <c r="F15" s="88" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="G15" s="90" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="H15" s="55"/>
     </row>
@@ -5723,15 +5720,15 @@
       <c r="A16" s="55"/>
       <c r="B16" s="43"/>
       <c r="C16" s="65" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="D16" s="55"/>
       <c r="E16" s="55"/>
       <c r="F16" s="88" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="G16" s="76" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="H16" s="55"/>
     </row>
@@ -5739,12 +5736,12 @@
       <c r="A17" s="55"/>
       <c r="B17" s="43"/>
       <c r="C17" s="55" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="D17" s="55"/>
       <c r="E17" s="55"/>
       <c r="F17" s="88" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="G17" s="76" t="s">
         <v>160</v>
@@ -5754,16 +5751,16 @@
     <row r="18" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A18" s="55"/>
       <c r="B18" s="66" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="C18" s="55"/>
       <c r="D18" s="55"/>
       <c r="E18" s="55"/>
       <c r="F18" s="88" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="G18" s="90" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="H18" s="55"/>
     </row>
@@ -5778,7 +5775,7 @@
     </row>
     <row r="20" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A20" s="75" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="B20" s="75"/>
       <c r="C20" s="57"/>
@@ -5792,15 +5789,15 @@
       <c r="A21" s="55"/>
       <c r="B21" s="43"/>
       <c r="C21" s="55" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="D21" s="55"/>
       <c r="E21" s="55"/>
       <c r="F21" s="88" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="G21" s="90" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="H21" s="55"/>
     </row>
@@ -5808,7 +5805,7 @@
       <c r="A22" s="55"/>
       <c r="B22" s="43"/>
       <c r="C22" s="55" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="D22" s="55"/>
       <c r="E22" s="55"/>
@@ -5820,11 +5817,11 @@
       <c r="B23" s="43"/>
       <c r="C23" s="55"/>
       <c r="D23" s="49" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="E23" s="55"/>
       <c r="F23" s="88" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="G23" s="76" t="s">
         <v>154</v>
@@ -5836,14 +5833,14 @@
       <c r="B24" s="43"/>
       <c r="C24" s="55"/>
       <c r="D24" s="49" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="E24" s="55"/>
       <c r="F24" s="88" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="G24" s="90" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="H24" s="43"/>
     </row>
@@ -5852,14 +5849,14 @@
       <c r="B25" s="43"/>
       <c r="C25" s="55"/>
       <c r="D25" s="49" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="E25" s="55"/>
       <c r="F25" s="88" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="G25" s="90" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="H25" s="55"/>
     </row>
@@ -5868,11 +5865,11 @@
       <c r="B26" s="43"/>
       <c r="C26" s="55"/>
       <c r="D26" s="49" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="E26" s="55"/>
       <c r="F26" s="88" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="G26" s="76" t="s">
         <v>156</v>
@@ -5884,11 +5881,11 @@
       <c r="B27" s="43"/>
       <c r="C27" s="55"/>
       <c r="D27" s="49" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="E27" s="55"/>
       <c r="F27" s="88" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="G27" s="76" t="s">
         <v>159</v>
@@ -5900,14 +5897,14 @@
       <c r="B28" s="43"/>
       <c r="C28" s="55"/>
       <c r="D28" s="49" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="E28" s="55"/>
       <c r="F28" s="88" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="G28" s="90" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="H28" s="55"/>
     </row>
@@ -5916,14 +5913,14 @@
       <c r="B29" s="43"/>
       <c r="C29" s="55"/>
       <c r="D29" s="49" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="E29" s="55"/>
       <c r="F29" s="88" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="G29" s="90" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="H29" s="55"/>
     </row>
@@ -5942,7 +5939,7 @@
       <c r="A31" s="55"/>
       <c r="B31" s="43"/>
       <c r="C31" s="55" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D31" s="55"/>
       <c r="E31" s="55"/>
@@ -5954,11 +5951,11 @@
       <c r="B32" s="43"/>
       <c r="C32" s="55"/>
       <c r="D32" s="49" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="E32" s="55"/>
       <c r="F32" s="88" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="G32" s="76" t="s">
         <v>249</v>
@@ -5970,14 +5967,14 @@
       <c r="B33" s="43"/>
       <c r="C33" s="55"/>
       <c r="D33" s="49" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="E33" s="55"/>
       <c r="F33" s="88" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="G33" s="90" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="H33" s="55"/>
     </row>
@@ -5986,11 +5983,11 @@
       <c r="B34" s="43"/>
       <c r="C34" s="55"/>
       <c r="D34" s="49" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="E34" s="55"/>
       <c r="F34" s="88" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="G34" s="76" t="s">
         <v>241</v>
@@ -6002,14 +5999,14 @@
       <c r="B35" s="43"/>
       <c r="C35" s="55"/>
       <c r="D35" s="49" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="E35" s="55"/>
       <c r="F35" s="88" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="G35" s="90" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="H35" s="55"/>
     </row>
@@ -6018,14 +6015,14 @@
       <c r="B36" s="43"/>
       <c r="C36" s="55"/>
       <c r="D36" s="49" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="E36" s="55"/>
       <c r="F36" s="88" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="G36" s="90" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="H36" s="55"/>
     </row>
@@ -6034,14 +6031,14 @@
       <c r="B37" s="43"/>
       <c r="C37" s="55"/>
       <c r="D37" s="49" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="E37" s="55"/>
       <c r="F37" s="88" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="G37" s="90" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="H37" s="55"/>
     </row>
@@ -6050,14 +6047,14 @@
       <c r="B38" s="43"/>
       <c r="C38" s="55"/>
       <c r="D38" s="49" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="E38" s="55"/>
       <c r="F38" s="88" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="G38" s="90" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="H38" s="55"/>
     </row>
@@ -6066,14 +6063,14 @@
       <c r="B39" s="43"/>
       <c r="C39" s="55"/>
       <c r="D39" s="49" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="E39" s="55"/>
       <c r="F39" s="88" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="G39" s="90" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="H39" s="43"/>
     </row>
@@ -6082,11 +6079,11 @@
       <c r="B40" s="43"/>
       <c r="C40" s="55"/>
       <c r="D40" s="49" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="E40" s="55"/>
       <c r="F40" s="88" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="G40" s="76" t="s">
         <v>248</v>
@@ -6098,14 +6095,14 @@
       <c r="B41" s="43"/>
       <c r="C41" s="55"/>
       <c r="D41" s="49" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="E41" s="55"/>
       <c r="F41" s="88" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="G41" s="91" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="H41" s="43"/>
     </row>
@@ -6113,31 +6110,31 @@
       <c r="A42" s="55"/>
       <c r="B42" s="43"/>
       <c r="C42" s="69" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="D42" s="55"/>
       <c r="E42" s="55"/>
       <c r="F42" s="88" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="G42" s="91" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="H42" s="43"/>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A43" s="55"/>
       <c r="B43" s="70" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="C43" s="55"/>
       <c r="D43" s="55"/>
       <c r="E43" s="55"/>
       <c r="F43" s="88" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="G43" s="91" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="H43" s="43"/>
     </row>
@@ -6153,7 +6150,7 @@
     </row>
     <row r="45" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A45" s="57" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="B45" s="57"/>
       <c r="C45" s="57"/>
@@ -6166,7 +6163,7 @@
     <row r="46" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A46" s="43"/>
       <c r="B46" s="66" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="C46" s="43"/>
       <c r="D46" s="43"/>
@@ -6178,15 +6175,15 @@
       <c r="A47" s="43"/>
       <c r="B47" s="43"/>
       <c r="C47" s="49" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="D47" s="43"/>
       <c r="E47" s="88" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="F47" s="43"/>
       <c r="G47" s="90" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="H47" s="43"/>
     </row>
@@ -6194,17 +6191,17 @@
       <c r="A48" s="43"/>
       <c r="B48" s="43"/>
       <c r="C48" s="49" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="D48" s="43"/>
       <c r="E48" s="88" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="F48" s="88" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="G48" s="90" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="H48" s="43"/>
     </row>
@@ -6217,16 +6214,16 @@
     <row r="50" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A50" s="43"/>
       <c r="B50" s="70" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="C50" s="43"/>
       <c r="D50" s="43"/>
       <c r="E50" s="43"/>
       <c r="F50" s="88" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="G50" s="90" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.35">
@@ -6240,14 +6237,14 @@
     <row r="52" spans="1:7" s="77" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A52" s="55"/>
       <c r="B52" s="66" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="G52" s="90"/>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A53" s="43"/>
       <c r="C53" s="49" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="D53" s="43"/>
       <c r="E53" s="43"/>
@@ -6258,14 +6255,14 @@
       <c r="B54" s="43"/>
       <c r="C54" s="43"/>
       <c r="D54" s="55" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="E54" s="88" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="F54" s="43"/>
       <c r="G54" s="90" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.35">
@@ -6273,14 +6270,14 @@
       <c r="B55" s="55"/>
       <c r="C55" s="67"/>
       <c r="D55" s="55" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="E55" s="88" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="F55" s="67"/>
       <c r="G55" s="90" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.35">
@@ -6288,165 +6285,165 @@
       <c r="B56" s="55"/>
       <c r="C56" s="67"/>
       <c r="D56" s="55" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="E56" s="88" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="F56" s="88" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="G56" s="90" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A57" s="67"/>
       <c r="B57" s="55"/>
       <c r="C57" s="49" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="D57" s="43"/>
       <c r="F57" s="88" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="G57" s="90" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A58" s="43"/>
       <c r="B58" s="43"/>
       <c r="C58" s="49" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="D58" s="43"/>
       <c r="E58" s="43"/>
       <c r="F58" s="88" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="G58" s="90" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A59" s="43"/>
       <c r="B59" s="43"/>
       <c r="C59" s="49" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="D59" s="43"/>
       <c r="E59" s="43"/>
       <c r="F59" s="88" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="G59" s="90" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A60" s="43"/>
       <c r="B60" s="43"/>
       <c r="C60" s="49" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="D60" s="43"/>
       <c r="E60" s="43"/>
       <c r="F60" s="88" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="G60" s="90" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A61" s="43"/>
       <c r="B61" s="43"/>
       <c r="C61" s="49" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="D61" s="43"/>
       <c r="E61" s="43"/>
       <c r="F61" s="88" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="G61" s="90" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A62" s="43"/>
       <c r="B62" s="43"/>
       <c r="C62" s="49" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="D62" s="43"/>
       <c r="E62" s="43"/>
       <c r="F62" s="88" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="G62" s="90" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A63" s="43"/>
       <c r="B63" s="43"/>
       <c r="C63" s="49" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="D63" s="43"/>
       <c r="E63" s="43"/>
       <c r="F63" s="88" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="G63" s="90" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A64" s="43"/>
       <c r="B64" s="43"/>
       <c r="C64" s="49" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="D64" s="43"/>
       <c r="E64" s="43"/>
       <c r="F64" s="88" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="G64" s="90" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A65" s="43"/>
       <c r="B65" s="43"/>
       <c r="C65" s="49" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="D65" s="43"/>
       <c r="E65" s="43"/>
       <c r="F65" s="88" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="G65" s="90" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A66" s="43"/>
       <c r="B66" s="43"/>
       <c r="C66" s="49" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="D66" s="43"/>
       <c r="E66" s="43"/>
       <c r="F66" s="89" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="G66" s="90" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.35">
@@ -6460,16 +6457,16 @@
     <row r="68" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A68" s="43"/>
       <c r="B68" s="71" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="C68" s="43"/>
       <c r="D68" s="43"/>
       <c r="E68" s="43"/>
       <c r="F68" s="88" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="G68" s="90" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.35">
@@ -6483,7 +6480,7 @@
     <row r="70" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A70" s="43"/>
       <c r="B70" s="66" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="C70" s="43"/>
       <c r="D70" s="43"/>
@@ -6494,135 +6491,135 @@
       <c r="A71" s="43"/>
       <c r="B71" s="43"/>
       <c r="C71" s="65" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="D71" s="43"/>
       <c r="E71" s="43"/>
       <c r="F71" s="88" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="G71" s="90" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A72" s="43"/>
       <c r="B72" s="43"/>
       <c r="C72" s="65" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="D72" s="43"/>
       <c r="E72" s="43"/>
       <c r="F72" s="88" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="G72" s="90" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A73" s="43"/>
       <c r="B73" s="43"/>
       <c r="C73" s="65" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="D73" s="43"/>
       <c r="E73" s="43"/>
       <c r="F73" s="88" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="G73" s="90" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A74" s="43"/>
       <c r="B74" s="43"/>
       <c r="C74" s="65" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="D74" s="43"/>
       <c r="E74" s="43"/>
       <c r="F74" s="88" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="G74" s="90" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A75" s="43"/>
       <c r="B75" s="43"/>
       <c r="C75" s="65" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="D75" s="43"/>
       <c r="E75" s="43"/>
       <c r="F75" s="88" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="G75" s="90" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A76" s="43"/>
       <c r="B76" s="43"/>
       <c r="C76" s="65" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="D76" s="43"/>
       <c r="E76" s="43"/>
       <c r="F76" s="88" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="G76" s="90" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A77" s="43"/>
       <c r="B77" s="43"/>
       <c r="C77" s="65" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="D77" s="43"/>
       <c r="E77" s="43"/>
       <c r="F77" s="88" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="G77" s="90" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A78" s="43"/>
       <c r="B78" s="43"/>
       <c r="C78" s="65" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="D78" s="43"/>
       <c r="E78" s="43"/>
       <c r="F78" s="88" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="G78" s="90" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A79" s="43"/>
       <c r="B79" s="71" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="C79" s="43"/>
       <c r="D79" s="43"/>
       <c r="E79" s="43"/>
       <c r="F79" s="88" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="G79" s="90" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.35">
@@ -6636,52 +6633,52 @@
     <row r="81" spans="1:7" s="77" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A81" s="55"/>
       <c r="B81" s="71" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="G81" s="90"/>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A82" s="43"/>
       <c r="C82" s="65" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="D82" s="43"/>
       <c r="E82" s="43"/>
       <c r="F82" s="88" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="G82" s="90" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A83" s="43"/>
       <c r="B83" s="43"/>
       <c r="C83" s="65" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="D83" s="43"/>
       <c r="E83" s="43"/>
       <c r="F83" s="88" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="G83" s="90" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A84" s="43"/>
       <c r="B84" s="43"/>
       <c r="C84" s="65" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="D84" s="43"/>
       <c r="E84" s="43"/>
       <c r="F84" s="89" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="G84" s="90" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.35">
@@ -6695,16 +6692,16 @@
     <row r="86" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A86" s="43"/>
       <c r="B86" s="71" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="C86" s="43"/>
       <c r="D86" s="43"/>
       <c r="E86" s="43"/>
       <c r="F86" s="88" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="G86" s="90" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.35">
@@ -6718,37 +6715,37 @@
     <row r="88" spans="1:7" s="77" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A88" s="65"/>
       <c r="B88" s="71" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="G88" s="90"/>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A89" s="43"/>
       <c r="C89" s="65" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="D89" s="43"/>
       <c r="E89" s="43"/>
       <c r="F89" s="89" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="G89" s="90" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A90" s="43"/>
       <c r="B90" s="43"/>
       <c r="C90" s="65" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="D90" s="43"/>
       <c r="E90" s="43"/>
       <c r="F90" s="89" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="G90" s="90" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.35">
@@ -6762,16 +6759,16 @@
     <row r="92" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A92" s="43"/>
       <c r="B92" s="71" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="C92" s="43"/>
       <c r="D92" s="43"/>
       <c r="E92" s="43"/>
       <c r="F92" s="88" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="G92" s="90" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.35">
@@ -6785,7 +6782,7 @@
     <row r="94" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A94" s="43"/>
       <c r="B94" s="71" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="C94" s="43"/>
       <c r="D94" s="43"/>
@@ -6796,50 +6793,50 @@
       <c r="A95" s="43"/>
       <c r="B95" s="43"/>
       <c r="C95" s="65" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="D95" s="43"/>
       <c r="E95" s="43"/>
       <c r="F95" s="88" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="G95" s="90" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A96" s="43"/>
       <c r="B96" s="66" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="C96" s="43"/>
       <c r="D96" s="43"/>
       <c r="E96" s="43"/>
       <c r="F96" s="88" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="G96" s="90" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A97" s="43"/>
       <c r="B97" s="66" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="C97" s="43"/>
       <c r="D97" s="43"/>
       <c r="E97" s="43"/>
       <c r="F97" s="88" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="G97" s="90" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
     </row>
     <row r="99" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A99" s="57" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="B99" s="57"/>
       <c r="C99" s="74"/>
@@ -6850,16 +6847,16 @@
     <row r="100" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A100" s="43"/>
       <c r="B100" s="55" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="C100" s="43"/>
       <c r="D100" s="43"/>
       <c r="E100" s="43"/>
       <c r="F100" s="88" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="G100" s="90" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.35">
@@ -6875,146 +6872,146 @@
       <c r="B102" s="43"/>
       <c r="C102" s="43"/>
       <c r="D102" s="72" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="E102" s="43"/>
       <c r="F102" s="88" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="G102" s="90" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B103" s="43"/>
       <c r="C103" s="43"/>
       <c r="D103" s="72" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="E103" s="43"/>
       <c r="F103" s="88" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="G103" s="90" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B104" s="43"/>
       <c r="C104" s="43"/>
       <c r="D104" s="72" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="E104" s="43"/>
       <c r="F104" s="88" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="G104" s="90" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B105" s="43"/>
       <c r="C105" s="43"/>
       <c r="D105" s="72" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="E105" s="43"/>
       <c r="F105" s="88" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="G105" s="90" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B106" s="43"/>
       <c r="C106" s="43"/>
       <c r="D106" s="72" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="E106" s="43"/>
       <c r="F106" s="88" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="G106" s="90" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B107" s="43"/>
       <c r="C107" s="43"/>
       <c r="D107" s="72" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="E107" s="43"/>
       <c r="F107" s="88" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="G107" s="90" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B108" s="43"/>
       <c r="C108" s="43"/>
       <c r="D108" s="72" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="E108" s="43"/>
       <c r="F108" s="88" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="G108" s="90" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B109" s="43"/>
       <c r="C109" s="43"/>
       <c r="D109" s="72" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="E109" s="43"/>
       <c r="F109" s="88" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="G109" s="90" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B110" s="70" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="C110" s="43"/>
       <c r="D110" s="43"/>
       <c r="E110" s="43"/>
       <c r="F110" s="88" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="G110" s="90" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B111" s="55" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="C111" s="43"/>
       <c r="D111" s="43"/>
       <c r="E111" s="43"/>
       <c r="F111" s="88" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="G111" s="90" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B112" s="43"/>
       <c r="C112" s="73" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="D112" s="43"/>
       <c r="E112" s="43"/>
@@ -7024,14 +7021,14 @@
       <c r="B113" s="43"/>
       <c r="C113" s="43"/>
       <c r="D113" s="72" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="E113" s="43"/>
       <c r="F113" s="88" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="G113" s="90" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.35">
@@ -7047,48 +7044,48 @@
       <c r="B115" s="43"/>
       <c r="C115" s="43"/>
       <c r="D115" s="55" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="E115" s="43"/>
       <c r="F115" s="88" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="G115" s="90" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
     </row>
     <row r="116" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B116" s="70" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="C116" s="43"/>
       <c r="D116" s="43"/>
       <c r="E116" s="43"/>
       <c r="F116" s="88" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="G116" s="90" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
     </row>
     <row r="117" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A117" s="43"/>
       <c r="B117" s="70" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="C117" s="43"/>
       <c r="D117" s="43"/>
       <c r="E117" s="43"/>
       <c r="F117" s="88" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="G117" s="90" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
     </row>
     <row r="119" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A119" s="57" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="B119" s="57"/>
       <c r="C119" s="74"/>
@@ -7099,7 +7096,7 @@
     <row r="120" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A120" s="43"/>
       <c r="B120" s="55" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="C120" s="43"/>
       <c r="D120" s="43"/>
@@ -7110,12 +7107,12 @@
       <c r="A121" s="43"/>
       <c r="B121" s="43"/>
       <c r="C121" s="72" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="D121" s="43"/>
       <c r="E121" s="43"/>
       <c r="F121" s="88" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="G121" s="90" t="s">
         <v>262</v>
@@ -7125,15 +7122,15 @@
       <c r="A122" s="43"/>
       <c r="B122" s="43"/>
       <c r="C122" s="72" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="D122" s="43"/>
       <c r="E122" s="43"/>
       <c r="F122" s="88" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="G122" s="90" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
     </row>
     <row r="123" spans="1:7" x14ac:dyDescent="0.35">
@@ -7150,22 +7147,22 @@
       <c r="A124" s="43"/>
       <c r="B124" s="43"/>
       <c r="C124" s="72" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="D124" s="43"/>
       <c r="E124" s="43"/>
       <c r="F124" s="88" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="G124" s="91" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
     </row>
     <row r="125" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A125" s="43"/>
       <c r="B125" s="43"/>
       <c r="C125" s="72" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="D125" s="43"/>
       <c r="E125" s="43"/>
@@ -7176,14 +7173,14 @@
       <c r="B126" s="43"/>
       <c r="C126" s="43"/>
       <c r="D126" s="72" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="E126" s="88" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="F126" s="43"/>
       <c r="G126" s="90" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
     </row>
     <row r="127" spans="1:7" x14ac:dyDescent="0.35">
@@ -7191,91 +7188,91 @@
       <c r="B127" s="43"/>
       <c r="C127" s="43"/>
       <c r="D127" s="72" t="s">
+        <v>514</v>
+      </c>
+      <c r="E127" s="88" t="s">
+        <v>536</v>
+      </c>
+      <c r="F127" s="88" t="s">
+        <v>644</v>
+      </c>
+      <c r="G127" s="90" t="s">
         <v>515</v>
-      </c>
-      <c r="E127" s="88" t="s">
-        <v>537</v>
-      </c>
-      <c r="F127" s="88" t="s">
-        <v>645</v>
-      </c>
-      <c r="G127" s="90" t="s">
-        <v>516</v>
       </c>
     </row>
     <row r="128" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A128" s="43"/>
       <c r="B128" s="43"/>
       <c r="C128" s="72" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="D128" s="43"/>
       <c r="E128" s="43"/>
       <c r="F128" s="88" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="G128" s="90" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
     </row>
     <row r="129" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A129" s="43"/>
       <c r="B129" s="43"/>
       <c r="C129" s="56" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="D129" s="43"/>
       <c r="E129" s="43"/>
       <c r="F129" s="88" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="G129" s="90" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
     </row>
     <row r="130" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A130" s="43"/>
       <c r="B130" s="70" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="C130" s="43"/>
       <c r="D130" s="43"/>
       <c r="E130" s="43"/>
       <c r="F130" s="88" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="G130" s="90" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
     </row>
     <row r="131" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A131" s="43"/>
       <c r="B131" s="70" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="C131" s="43"/>
       <c r="D131" s="43"/>
       <c r="E131" s="43"/>
       <c r="F131" s="88" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="G131" s="90" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
     </row>
     <row r="132" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A132" s="43"/>
       <c r="B132" s="72" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="C132" s="43"/>
       <c r="D132" s="43"/>
       <c r="E132" s="43"/>
       <c r="F132" s="88" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="G132" s="90" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
     </row>
   </sheetData>
@@ -7303,7 +7300,7 @@
   <sheetData>
     <row r="1" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="85" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="B1" s="78"/>
       <c r="C1" s="78"/>
@@ -7314,51 +7311,51 @@
     </row>
     <row r="2" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="86" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="B2" s="79"/>
       <c r="C2" s="80"/>
       <c r="D2" s="79"/>
       <c r="E2" s="77" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="86" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="B3" s="80"/>
       <c r="C3" s="80"/>
       <c r="D3" s="80"/>
       <c r="E3" s="77" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="86" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="B4" s="80"/>
       <c r="C4" s="80"/>
       <c r="D4" s="80"/>
       <c r="E4" s="77" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="86" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="B5" s="80"/>
       <c r="C5" s="80"/>
       <c r="D5" s="80"/>
       <c r="E5" s="77" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="86" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="B6" s="80"/>
       <c r="C6" s="80"/>
@@ -7367,18 +7364,18 @@
     </row>
     <row r="7" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A7" s="86" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="B7" s="81"/>
       <c r="C7" s="81"/>
       <c r="D7" s="82"/>
       <c r="E7" s="77" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A8" s="86" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="B8" s="83"/>
       <c r="C8" s="83"/>
@@ -7404,8 +7401,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A4:G98"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScale="82" workbookViewId="0">
-      <selection activeCell="F57" sqref="F57"/>
+    <sheetView zoomScale="82" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -7426,51 +7423,51 @@
         <v>285</v>
       </c>
       <c r="G4" t="s">
-        <v>286</v>
+        <v>152</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" s="25" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B6" s="27" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="C7" s="27" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="D7" s="27"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="D8" s="28" t="s">
+        <v>289</v>
+      </c>
+      <c r="E8" s="88" t="s">
+        <v>536</v>
+      </c>
+      <c r="F8" s="88" t="s">
+        <v>536</v>
+      </c>
+      <c r="G8" t="s">
         <v>290</v>
-      </c>
-      <c r="E8" s="88" t="s">
-        <v>537</v>
-      </c>
-      <c r="F8" s="88" t="s">
-        <v>537</v>
-      </c>
-      <c r="G8" t="s">
-        <v>291</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="D9" s="28" t="s">
+        <v>291</v>
+      </c>
+      <c r="E9" s="88" t="s">
+        <v>536</v>
+      </c>
+      <c r="F9" s="88" t="s">
+        <v>536</v>
+      </c>
+      <c r="G9" t="s">
         <v>292</v>
-      </c>
-      <c r="E9" s="88" t="s">
-        <v>537</v>
-      </c>
-      <c r="F9" s="88" t="s">
-        <v>537</v>
-      </c>
-      <c r="G9" t="s">
-        <v>293</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.35">
@@ -7481,50 +7478,50 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="C11" s="30" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="D11" s="30"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="D12" s="31" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="E12" s="88" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="F12" s="88" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="G12" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="D13" s="31" t="s">
+        <v>295</v>
+      </c>
+      <c r="E13" s="88" t="s">
+        <v>536</v>
+      </c>
+      <c r="F13" s="88" t="s">
+        <v>536</v>
+      </c>
+      <c r="G13" t="s">
         <v>296</v>
-      </c>
-      <c r="E13" s="88" t="s">
-        <v>537</v>
-      </c>
-      <c r="F13" s="88" t="s">
-        <v>537</v>
-      </c>
-      <c r="G13" t="s">
-        <v>297</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="D14" s="31" t="s">
+        <v>297</v>
+      </c>
+      <c r="E14" s="88" t="s">
+        <v>536</v>
+      </c>
+      <c r="F14" s="88" t="s">
+        <v>536</v>
+      </c>
+      <c r="G14" t="s">
         <v>298</v>
-      </c>
-      <c r="E14" s="88" t="s">
-        <v>537</v>
-      </c>
-      <c r="F14" s="88" t="s">
-        <v>537</v>
-      </c>
-      <c r="G14" t="s">
-        <v>299</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.35">
@@ -7535,106 +7532,106 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B16" s="33" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="D16" s="33"/>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.35">
       <c r="C17" s="32" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D17" s="32"/>
       <c r="E17" s="88" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="F17" s="88" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="G17" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.35">
       <c r="C18" s="32" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D18" s="32"/>
       <c r="E18" s="88" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="F18" s="88" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="G18" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.35">
       <c r="C19" s="32" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="D19" s="32"/>
       <c r="E19" s="88" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="F19" s="88" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="G19" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.35">
       <c r="C20" s="32" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="D20" s="32"/>
       <c r="E20" s="88" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="F20" s="88" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="G20" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.35">
       <c r="C21" s="30" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="D21" s="30"/>
       <c r="E21" s="88" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="F21" s="88" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="G21" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.35">
       <c r="C22" s="30"/>
       <c r="D22" s="30" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="E22" s="29"/>
       <c r="F22" s="29"/>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B23" s="30" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D23" s="30"/>
       <c r="E23" s="88" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="F23" s="88" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="G23" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.35">
@@ -7645,7 +7642,7 @@
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B25" s="30" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="D25" s="30"/>
       <c r="E25" s="29"/>
@@ -7653,7 +7650,7 @@
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.35">
       <c r="C26" s="30" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="D26" s="30"/>
       <c r="E26" s="34">
@@ -7663,12 +7660,12 @@
         <v>7000.1</v>
       </c>
       <c r="G26" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.35">
       <c r="C27" s="30" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="D27" s="30"/>
       <c r="E27" s="35">
@@ -7678,7 +7675,7 @@
         <v>7000.2</v>
       </c>
       <c r="G27" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.35">
@@ -7689,7 +7686,7 @@
     </row>
     <row r="29" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B29" s="30" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="D29" s="30"/>
       <c r="E29" s="29"/>
@@ -7697,7 +7694,7 @@
     </row>
     <row r="30" spans="2:7" x14ac:dyDescent="0.35">
       <c r="C30" s="30" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="D30" s="30"/>
       <c r="E30" s="36">
@@ -7707,12 +7704,12 @@
         <v>7000.4</v>
       </c>
       <c r="G30" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="31" spans="2:7" x14ac:dyDescent="0.35">
       <c r="C31" s="30" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="D31" s="30"/>
       <c r="E31" s="35">
@@ -7722,7 +7719,7 @@
         <v>7000.5</v>
       </c>
       <c r="G31" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="32" spans="2:7" x14ac:dyDescent="0.35">
@@ -7733,7 +7730,7 @@
     </row>
     <row r="33" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B33" s="30" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="D33" s="30"/>
       <c r="E33" s="36">
@@ -7743,7 +7740,7 @@
         <v>7000.6</v>
       </c>
       <c r="G33" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="34" spans="2:7" x14ac:dyDescent="0.35">
@@ -7754,7 +7751,7 @@
     </row>
     <row r="35" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B35" s="30" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="D35" s="30"/>
       <c r="E35" s="36">
@@ -7764,7 +7761,7 @@
         <v>7000.7</v>
       </c>
       <c r="G35" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="36" spans="2:7" x14ac:dyDescent="0.35">
@@ -7775,7 +7772,7 @@
     </row>
     <row r="37" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B37" s="30" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="D37" s="30"/>
       <c r="E37" s="29"/>
@@ -7783,7 +7780,7 @@
     </row>
     <row r="38" spans="2:7" x14ac:dyDescent="0.35">
       <c r="C38" s="30" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="D38" s="30"/>
       <c r="E38" s="37">
@@ -7793,12 +7790,12 @@
         <v>7000.8</v>
       </c>
       <c r="G38" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="39" spans="2:7" x14ac:dyDescent="0.35">
       <c r="C39" s="30" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D39" s="30"/>
       <c r="E39" s="35">
@@ -7808,7 +7805,7 @@
         <v>7000.9</v>
       </c>
       <c r="G39" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="40" spans="2:7" x14ac:dyDescent="0.35">
@@ -7819,17 +7816,17 @@
     </row>
     <row r="41" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B41" s="30" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="D41" s="30"/>
       <c r="E41" s="88" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="F41" s="88" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="G41" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="42" spans="2:7" x14ac:dyDescent="0.35">
@@ -7840,7 +7837,7 @@
     </row>
     <row r="43" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B43" s="30" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="D43" s="30"/>
       <c r="E43" s="29"/>
@@ -7848,22 +7845,22 @@
     </row>
     <row r="44" spans="2:7" x14ac:dyDescent="0.35">
       <c r="C44" s="30" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="D44" s="30"/>
       <c r="E44" s="88" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="F44" s="88" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="G44" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="45" spans="2:7" x14ac:dyDescent="0.35">
       <c r="C45" s="30" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="D45" s="30"/>
       <c r="E45" s="35">
@@ -7873,7 +7870,7 @@
         <v>7400.2</v>
       </c>
       <c r="G45" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="46" spans="2:7" x14ac:dyDescent="0.35">
@@ -7884,7 +7881,7 @@
     </row>
     <row r="47" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B47" s="30" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="D47" s="30"/>
       <c r="E47" s="36">
@@ -7894,7 +7891,7 @@
         <v>7400.1</v>
       </c>
       <c r="G47" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="48" spans="2:7" x14ac:dyDescent="0.35">
@@ -7905,95 +7902,95 @@
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B49" s="30" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="D49" s="30"/>
       <c r="E49" s="38" t="s">
+        <v>341</v>
+      </c>
+      <c r="F49" s="38" t="s">
+        <v>341</v>
+      </c>
+      <c r="G49" t="s">
         <v>342</v>
-      </c>
-      <c r="F49" s="38" t="s">
-        <v>342</v>
-      </c>
-      <c r="G49" t="s">
-        <v>343</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.35">
       <c r="C50" s="39"/>
       <c r="D50" s="30"/>
       <c r="E50" s="88" t="s">
+        <v>536</v>
+      </c>
+      <c r="F50" s="88" t="s">
+        <v>536</v>
+      </c>
+      <c r="G50" s="77" t="s">
         <v>537</v>
-      </c>
-      <c r="F50" s="88" t="s">
-        <v>537</v>
-      </c>
-      <c r="G50" s="77" t="s">
-        <v>538</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.35">
       <c r="C51" s="40"/>
       <c r="D51" s="30"/>
       <c r="E51" s="88" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="F51" s="88" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="G51" s="77" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.35">
       <c r="C52" s="40"/>
       <c r="D52" s="30"/>
       <c r="E52" s="88" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="F52" s="88" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="G52" s="77" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.35">
       <c r="C53" s="40"/>
       <c r="D53" s="30"/>
       <c r="E53" s="88" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="F53" s="88" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="G53" s="77" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.35">
       <c r="C54" s="40"/>
       <c r="D54" s="30"/>
       <c r="E54" s="88" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="F54" s="88" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="G54" s="77" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.35">
       <c r="C55" s="40"/>
       <c r="D55" s="30"/>
       <c r="E55" s="88" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="F55" s="88" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="G55" s="77" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.35">
@@ -8005,37 +8002,37 @@
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A57" s="41" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="D57" s="41"/>
       <c r="E57" s="88" t="s">
+        <v>647</v>
+      </c>
+      <c r="F57" s="88" t="s">
         <v>648</v>
       </c>
-      <c r="F57" s="88" t="s">
-        <v>649</v>
-      </c>
       <c r="G57" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A59" s="25" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B60" s="27" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="D60" s="27"/>
       <c r="E60" s="88" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="F60" s="88" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="G60" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.35">
@@ -8044,17 +8041,17 @@
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B62" s="27" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="D62" s="27"/>
       <c r="E62" s="88" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="F62" s="88" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="G62" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.35">
@@ -8063,17 +8060,17 @@
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B64" s="27" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="D64" s="27"/>
       <c r="E64" s="88" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="F64" s="88" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="G64" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="65" spans="2:7" x14ac:dyDescent="0.35">
@@ -8082,53 +8079,53 @@
     </row>
     <row r="66" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B66" s="27" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="D66" s="27"/>
     </row>
     <row r="67" spans="2:7" x14ac:dyDescent="0.35">
       <c r="C67" s="27" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="D67" s="27"/>
       <c r="E67" s="88" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="F67" s="88" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="G67" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="68" spans="2:7" x14ac:dyDescent="0.35">
       <c r="C68" s="27" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="D68" s="27"/>
       <c r="E68" s="88" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="F68" s="88" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="G68" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="69" spans="2:7" x14ac:dyDescent="0.35">
       <c r="C69" s="27" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="D69" s="27"/>
       <c r="E69" s="88" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="F69" s="88" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="G69" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="70" spans="2:7" x14ac:dyDescent="0.35">
@@ -8137,38 +8134,38 @@
     </row>
     <row r="71" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B71" s="27" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="D71" s="27"/>
     </row>
     <row r="72" spans="2:7" x14ac:dyDescent="0.35">
       <c r="C72" s="27" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="D72" s="27"/>
       <c r="E72" s="88" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="F72" s="88" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="G72" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="73" spans="2:7" x14ac:dyDescent="0.35">
       <c r="C73" s="27" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="D73" s="27"/>
       <c r="E73" s="88" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="F73" s="88" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="G73" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="74" spans="2:7" x14ac:dyDescent="0.35">
@@ -8177,7 +8174,7 @@
     </row>
     <row r="75" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B75" s="27" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="D75" s="27"/>
       <c r="E75" s="36">
@@ -8187,7 +8184,7 @@
         <v>7420</v>
       </c>
       <c r="G75" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="76" spans="2:7" x14ac:dyDescent="0.35">
@@ -8196,17 +8193,17 @@
     </row>
     <row r="77" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B77" s="27" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="D77" s="27"/>
       <c r="E77" s="88" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="F77" s="88" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="G77" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="78" spans="2:7" x14ac:dyDescent="0.35">
@@ -8215,17 +8212,17 @@
     </row>
     <row r="79" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B79" s="27" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="D79" s="27"/>
       <c r="E79" s="88" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="F79" s="88" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="G79" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="80" spans="2:7" x14ac:dyDescent="0.35">
@@ -8234,17 +8231,17 @@
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B81" s="27" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="D81" s="27"/>
       <c r="E81" s="88" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="F81" s="88" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="G81" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.35">
@@ -8253,95 +8250,95 @@
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B83" s="27" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="D83" s="27"/>
       <c r="E83" s="88" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="F83" s="88" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="G83" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.35">
       <c r="C84" s="39"/>
       <c r="D84" s="30"/>
       <c r="E84" s="88" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="F84" s="88" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="G84" s="77" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.35">
       <c r="C85" s="39"/>
       <c r="D85" s="30"/>
       <c r="E85" s="88" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="F85" s="88" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="G85" s="77" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.35">
       <c r="C86" s="39"/>
       <c r="D86" s="30"/>
       <c r="E86" s="88" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="F86" s="88" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="G86" s="77" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.35">
       <c r="C87" s="39"/>
       <c r="D87" s="30"/>
       <c r="E87" s="88" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="F87" s="88" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="G87" s="77" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.35">
       <c r="C88" s="39"/>
       <c r="D88" s="30"/>
       <c r="E88" s="88" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="F88" s="88" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="G88" s="77" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.35">
       <c r="C89" s="39"/>
       <c r="D89" s="30"/>
       <c r="E89" s="89" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="F89" s="89" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="G89" s="77" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.35">
@@ -8358,17 +8355,17 @@
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A92" s="42" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="D92" s="42"/>
       <c r="E92" s="88" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="F92" s="88" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="G92" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.35">
@@ -8377,22 +8374,22 @@
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A94" s="27" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="D94" s="27"/>
       <c r="E94" s="88" t="s">
+        <v>651</v>
+      </c>
+      <c r="F94" s="88" t="s">
         <v>652</v>
       </c>
-      <c r="F94" s="88" t="s">
-        <v>653</v>
-      </c>
       <c r="G94" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A95" s="27" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="D95" s="27"/>
       <c r="E95" s="35">
@@ -8402,52 +8399,52 @@
         <v>7500</v>
       </c>
       <c r="G95" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A96" s="27" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="D96" s="27"/>
       <c r="E96" s="97" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="F96" s="97" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="G96" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A97" s="27" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="D97" s="27"/>
       <c r="E97" s="88" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="F97" s="88" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="G97" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A98" s="27" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="D98" s="27"/>
       <c r="E98" s="97" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="F98" s="97" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="G98" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
   </sheetData>

</xml_diff>